<commit_message>
chore: refresh global stats datasets from authenticated Fantacalcio xlsx
</commit_message>
<xml_diff>
--- a/data/reports/seriea_projection_round25_38.xlsx
+++ b/data/reports/seriea_projection_round25_38.xlsx
@@ -573,18 +573,18 @@
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr">
         <is>
-          <t>Kilicsoy</t>
+          <t>Mazzitelli</t>
         </is>
       </c>
       <c r="M2" t="inlineStr"/>
       <c r="N2" t="inlineStr">
         <is>
-          <t>Adopo; Caprile</t>
+          <t>Dossena; Obert</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>Falcone; Gallo</t>
+          <t>Ramadani; Gaspar K.</t>
         </is>
       </c>
       <c r="P2" t="inlineStr"/>
@@ -632,24 +632,24 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Baturina; Paz N.</t>
+          <t>Douvikas; Baturina</t>
         </is>
       </c>
       <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr">
         <is>
-          <t>Douvikas; Kempf</t>
+          <t>Rodriguez Je.; Paz N.</t>
         </is>
       </c>
       <c r="M3" t="inlineStr"/>
       <c r="N3" t="inlineStr">
         <is>
-          <t>Butez; Paz N.</t>
+          <t>Smolcic I.; Diego Carlos</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>De Gea; Dodò</t>
+          <t>Pongracic; Ranieri L.</t>
         </is>
       </c>
       <c r="P3" t="inlineStr"/>
@@ -702,27 +702,27 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>Malinovskyi</t>
+          <t>Colombo</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>Bonazzoli</t>
+          <t>Vandeputte</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>Ostigard</t>
+          <t>Martin</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>Baschirotto; Terracciano F.</t>
+          <t>Pezzella Giu.; Payero</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>Vasquez; Colombo</t>
+          <t>Gronbaek *; Malinovskyi</t>
         </is>
       </c>
       <c r="P4" t="inlineStr"/>
@@ -785,17 +785,17 @@
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>Bremer</t>
+          <t>Boga</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>Martinez L.; Barella</t>
+          <t>Calhanoglu; Barella</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>Kalulu</t>
+          <t>Gatti</t>
         </is>
       </c>
       <c r="P5" t="inlineStr"/>
@@ -847,17 +847,17 @@
       <c r="M6" t="inlineStr"/>
       <c r="N6" t="inlineStr">
         <is>
-          <t>Provedel; Gila</t>
+          <t>Taylor K.; Zaccagni</t>
         </is>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>Carnesecchi; De Ketelaere</t>
+          <t>Kolasinac; De Roon</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>Basic</t>
+          <t>Belahyane</t>
         </is>
       </c>
       <c r="Q6" t="inlineStr"/>
@@ -908,12 +908,12 @@
       <c r="M7" t="inlineStr"/>
       <c r="N7" t="inlineStr">
         <is>
-          <t>Di Lorenzo</t>
+          <t>Juan Jesus</t>
         </is>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>Svilar; Cristante</t>
+          <t>Zaragoza; Mancini</t>
         </is>
       </c>
       <c r="P7" t="inlineStr"/>
@@ -965,12 +965,12 @@
       <c r="M8" t="inlineStr"/>
       <c r="N8" t="inlineStr">
         <is>
-          <t>Bernabè; Pellegrino M.</t>
+          <t>Rinaldi; Nicolussi Caviglia</t>
         </is>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>Bernede; Nelsson</t>
+          <t>Akpa Akpro; Gagliardini</t>
         </is>
       </c>
       <c r="P8" t="inlineStr"/>
@@ -1025,17 +1025,17 @@
       <c r="L9" t="inlineStr"/>
       <c r="M9" t="inlineStr">
         <is>
-          <t>Rabiot; Nkunku</t>
+          <t>Rabiot; Athekame</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>Canestrelli; Aebischer</t>
+          <t>Coppola F.; Denoon</t>
         </is>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>Maignan; Saelemaekers</t>
+          <t>Athekame; Estupinan</t>
         </is>
       </c>
       <c r="P9" t="inlineStr"/>
@@ -1098,17 +1098,17 @@
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>Orsolini</t>
+          <t>Dominguez B.</t>
         </is>
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>Lazaro; Vlasic</t>
+          <t>Aboukhlal; Nkounkou</t>
         </is>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>Orsolini; Castro S.</t>
+          <t>De Silvestri; Lykogiannis</t>
         </is>
       </c>
       <c r="P10" t="inlineStr"/>
@@ -1166,22 +1166,22 @@
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>Zaniolo</t>
+          <t>Rui Modesto *</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>Volpato</t>
+          <t>Garcia U.</t>
         </is>
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>Karlstrom; Solet</t>
+          <t>Goglichidze *; Gueye</t>
         </is>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>Idzes; Laurientè</t>
+          <t>Iannoni; Thorstvedt</t>
         </is>
       </c>
       <c r="P11" t="inlineStr"/>
@@ -1229,32 +1229,32 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
+          <t>Scamacca</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>Santos A.</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
           <t>Raspadori</t>
         </is>
       </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>De Bruyne</t>
-        </is>
-      </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>Scamacca</t>
-        </is>
-      </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>Zambo Anguissa</t>
+          <t>Giovane</t>
         </is>
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>Carnesecchi; De Ketelaere</t>
+          <t>Kolasinac; De Roon</t>
         </is>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>Di Lorenzo</t>
+          <t>Juan Jesus</t>
         </is>
       </c>
       <c r="P12" t="inlineStr"/>
@@ -1312,22 +1312,22 @@
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>Orsolini</t>
+          <t>Dominguez B.</t>
         </is>
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>Zaniolo</t>
+          <t>Rui Modesto *</t>
         </is>
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>Orsolini; Castro S.</t>
+          <t>De Silvestri; Lykogiannis</t>
         </is>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>Karlstrom; Solet</t>
+          <t>Goglichidze *; Gueye</t>
         </is>
       </c>
       <c r="P13" t="inlineStr"/>
@@ -1376,29 +1376,29 @@
       <c r="J14" t="inlineStr"/>
       <c r="K14" t="inlineStr">
         <is>
-          <t>Castellanos *</t>
+          <t>Pedro</t>
         </is>
       </c>
       <c r="L14" t="inlineStr"/>
       <c r="M14" t="inlineStr">
         <is>
-          <t>Isaksen</t>
+          <t>Castellanos *</t>
         </is>
       </c>
       <c r="N14" t="inlineStr">
         <is>
-          <t>Adopo; Caprile</t>
+          <t>Dossena; Obert</t>
         </is>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>Provedel; Gila</t>
+          <t>Taylor K.; Zaccagni</t>
         </is>
       </c>
       <c r="P14" t="inlineStr"/>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>Basic</t>
+          <t>Belahyane</t>
         </is>
       </c>
       <c r="R14" t="n">
@@ -1444,24 +1444,24 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>Brescianini</t>
+          <t>Kean</t>
         </is>
       </c>
       <c r="K15" t="inlineStr"/>
       <c r="L15" t="inlineStr">
         <is>
-          <t>Mandragora</t>
+          <t>Harrison</t>
         </is>
       </c>
       <c r="M15" t="inlineStr"/>
       <c r="N15" t="inlineStr">
         <is>
-          <t>De Gea; Dodò</t>
+          <t>Pongracic; Ranieri L.</t>
         </is>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>Canestrelli; Aebischer</t>
+          <t>Coppola F.; Denoon</t>
         </is>
       </c>
       <c r="P15" t="inlineStr"/>
@@ -1509,7 +1509,7 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>Malinovskyi</t>
+          <t>Colombo</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
@@ -1519,7 +1519,7 @@
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>Ostigard</t>
+          <t>Martin</t>
         </is>
       </c>
       <c r="M16" t="inlineStr">
@@ -1529,12 +1529,12 @@
       </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t>Vasquez; Colombo</t>
+          <t>Gronbaek *; Malinovskyi</t>
         </is>
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>Lazaro; Vlasic</t>
+          <t>Aboukhlal; Nkounkou</t>
         </is>
       </c>
       <c r="P16" t="inlineStr"/>
@@ -1587,27 +1587,27 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
+          <t>Douvikas</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>Boga</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
           <t>Baturina</t>
         </is>
       </c>
-      <c r="L17" t="inlineStr">
-        <is>
-          <t>Bremer</t>
-        </is>
-      </c>
-      <c r="M17" t="inlineStr">
-        <is>
-          <t>Paz N.</t>
-        </is>
-      </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>Kalulu</t>
+          <t>Gatti</t>
         </is>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>Butez; Paz N.</t>
+          <t>Smolcic I.; Diego Carlos</t>
         </is>
       </c>
       <c r="P17" t="inlineStr"/>
@@ -1656,23 +1656,23 @@
       <c r="J18" t="inlineStr"/>
       <c r="K18" t="inlineStr">
         <is>
-          <t>Martinez L.; Dimarco</t>
+          <t>Martinez L.; Calhanoglu</t>
         </is>
       </c>
       <c r="L18" t="inlineStr"/>
       <c r="M18" t="inlineStr">
         <is>
-          <t>Calhanoglu; Bonny</t>
+          <t>Dimarco; Barella</t>
         </is>
       </c>
       <c r="N18" t="inlineStr">
         <is>
-          <t>Falcone; Gallo</t>
+          <t>Ramadani; Gaspar K.</t>
         </is>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>Martinez L.; Barella</t>
+          <t>Calhanoglu; Barella</t>
         </is>
       </c>
       <c r="P18" t="inlineStr"/>
@@ -1726,18 +1726,18 @@
       <c r="K19" t="inlineStr"/>
       <c r="L19" t="inlineStr">
         <is>
-          <t>Leao</t>
+          <t>Rabiot</t>
         </is>
       </c>
       <c r="M19" t="inlineStr"/>
       <c r="N19" t="inlineStr">
         <is>
-          <t>Maignan; Saelemaekers</t>
+          <t>Athekame; Estupinan</t>
         </is>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>Bernabè; Pellegrino M.</t>
+          <t>Rinaldi; Nicolussi Caviglia</t>
         </is>
       </c>
       <c r="P19" t="inlineStr"/>
@@ -1785,24 +1785,24 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>Soulè</t>
+          <t>Malen</t>
         </is>
       </c>
       <c r="K20" t="inlineStr"/>
       <c r="L20" t="inlineStr">
         <is>
-          <t>Malen</t>
+          <t>Zaragoza</t>
         </is>
       </c>
       <c r="M20" t="inlineStr"/>
       <c r="N20" t="inlineStr">
         <is>
-          <t>Svilar; Cristante</t>
+          <t>Zaragoza; Mancini</t>
         </is>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>Baschirotto; Terracciano F.</t>
+          <t>Pezzella Giu.; Payero</t>
         </is>
       </c>
       <c r="P20" t="inlineStr"/>
@@ -1856,18 +1856,18 @@
       <c r="K21" t="inlineStr"/>
       <c r="L21" t="inlineStr">
         <is>
-          <t>Volpato</t>
+          <t>Garcia U.</t>
         </is>
       </c>
       <c r="M21" t="inlineStr"/>
       <c r="N21" t="inlineStr">
         <is>
-          <t>Idzes; Laurientè</t>
+          <t>Iannoni; Thorstvedt</t>
         </is>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>Bernede; Nelsson</t>
+          <t>Akpa Akpro; Gagliardini</t>
         </is>
       </c>
       <c r="P21" t="inlineStr"/>
@@ -1915,24 +1915,24 @@
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>Baturina</t>
+          <t>Douvikas</t>
         </is>
       </c>
       <c r="K22" t="inlineStr"/>
       <c r="L22" t="inlineStr">
         <is>
-          <t>Paz N.</t>
+          <t>Baturina</t>
         </is>
       </c>
       <c r="M22" t="inlineStr"/>
       <c r="N22" t="inlineStr">
         <is>
-          <t>Butez; Paz N.</t>
+          <t>Smolcic I.; Diego Carlos</t>
         </is>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>Falcone; Gallo</t>
+          <t>Ramadani; Gaspar K.</t>
         </is>
       </c>
       <c r="P22" t="inlineStr"/>
@@ -1987,17 +1987,17 @@
       <c r="L23" t="inlineStr"/>
       <c r="M23" t="inlineStr">
         <is>
-          <t>Leao</t>
+          <t>Rabiot</t>
         </is>
       </c>
       <c r="N23" t="inlineStr">
         <is>
-          <t>Baschirotto; Terracciano F.</t>
+          <t>Pezzella Giu.; Payero</t>
         </is>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>Maignan; Saelemaekers</t>
+          <t>Athekame; Estupinan</t>
         </is>
       </c>
       <c r="P23" t="inlineStr"/>
@@ -2045,24 +2045,24 @@
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>Martinez L.; Dimarco; Calhanoglu</t>
+          <t>Martinez L.; Calhanoglu; Thuram</t>
         </is>
       </c>
       <c r="K24" t="inlineStr"/>
       <c r="L24" t="inlineStr">
         <is>
-          <t>Bonny; Thuram</t>
+          <t>Dimarco; Barella</t>
         </is>
       </c>
       <c r="M24" t="inlineStr"/>
       <c r="N24" t="inlineStr">
         <is>
-          <t>Martinez L.; Barella</t>
+          <t>Calhanoglu; Barella</t>
         </is>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>Vasquez; Colombo</t>
+          <t>Gronbaek *; Malinovskyi</t>
         </is>
       </c>
       <c r="P24" t="inlineStr"/>
@@ -2117,17 +2117,17 @@
       <c r="L25" t="inlineStr"/>
       <c r="M25" t="inlineStr">
         <is>
-          <t>Kilicsoy</t>
+          <t>Mazzitelli</t>
         </is>
       </c>
       <c r="N25" t="inlineStr">
         <is>
-          <t>Bernabè; Pellegrino M.</t>
+          <t>Rinaldi; Nicolussi Caviglia</t>
         </is>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>Adopo; Caprile</t>
+          <t>Dossena; Obert</t>
         </is>
       </c>
       <c r="P25" t="inlineStr"/>
@@ -2182,17 +2182,17 @@
       <c r="L26" t="inlineStr"/>
       <c r="M26" t="inlineStr">
         <is>
-          <t>Orsolini</t>
+          <t>Dominguez B.</t>
         </is>
       </c>
       <c r="N26" t="inlineStr">
         <is>
-          <t>Canestrelli; Aebischer</t>
+          <t>Coppola F.; Denoon</t>
         </is>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>Orsolini; Castro S.</t>
+          <t>De Silvestri; Lykogiannis</t>
         </is>
       </c>
       <c r="P26" t="inlineStr"/>
@@ -2244,12 +2244,12 @@
       <c r="M27" t="inlineStr"/>
       <c r="N27" t="inlineStr">
         <is>
-          <t>Svilar; Cristante</t>
+          <t>Zaragoza; Mancini</t>
         </is>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>Kalulu</t>
+          <t>Gatti</t>
         </is>
       </c>
       <c r="P27" t="inlineStr"/>
@@ -2298,23 +2298,23 @@
       <c r="J28" t="inlineStr"/>
       <c r="K28" t="inlineStr">
         <is>
-          <t>Raspadori</t>
+          <t>Scamacca</t>
         </is>
       </c>
       <c r="L28" t="inlineStr"/>
       <c r="M28" t="inlineStr">
         <is>
-          <t>Scamacca</t>
+          <t>Raspadori</t>
         </is>
       </c>
       <c r="N28" t="inlineStr">
         <is>
-          <t>Idzes; Laurientè</t>
+          <t>Iannoni; Thorstvedt</t>
         </is>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>Carnesecchi; De Ketelaere</t>
+          <t>Kolasinac; De Roon</t>
         </is>
       </c>
       <c r="P28" t="inlineStr"/>
@@ -2363,29 +2363,29 @@
       <c r="J29" t="inlineStr"/>
       <c r="K29" t="inlineStr">
         <is>
-          <t>Castellanos *</t>
+          <t>Pedro</t>
         </is>
       </c>
       <c r="L29" t="inlineStr"/>
       <c r="M29" t="inlineStr">
         <is>
-          <t>Isaksen</t>
+          <t>Castellanos *</t>
         </is>
       </c>
       <c r="N29" t="inlineStr">
         <is>
-          <t>Lazaro; Vlasic</t>
+          <t>Aboukhlal; Nkounkou</t>
         </is>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>Provedel; Gila</t>
+          <t>Taylor K.; Zaccagni</t>
         </is>
       </c>
       <c r="P29" t="inlineStr"/>
       <c r="Q29" t="inlineStr">
         <is>
-          <t>Basic</t>
+          <t>Belahyane</t>
         </is>
       </c>
       <c r="R29" t="n">
@@ -2436,27 +2436,27 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>Brescianini</t>
+          <t>Kean</t>
         </is>
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>Zaniolo</t>
+          <t>Rui Modesto *</t>
         </is>
       </c>
       <c r="M30" t="inlineStr">
         <is>
-          <t>Mandragora</t>
+          <t>Harrison</t>
         </is>
       </c>
       <c r="N30" t="inlineStr">
         <is>
-          <t>Karlstrom; Solet</t>
+          <t>Goglichidze *; Gueye</t>
         </is>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>De Gea; Dodò</t>
+          <t>Pongracic; Ranieri L.</t>
         </is>
       </c>
       <c r="P30" t="inlineStr"/>
@@ -2505,23 +2505,23 @@
       <c r="J31" t="inlineStr"/>
       <c r="K31" t="inlineStr">
         <is>
-          <t>De Bruyne</t>
+          <t>Santos A.</t>
         </is>
       </c>
       <c r="L31" t="inlineStr"/>
       <c r="M31" t="inlineStr">
         <is>
-          <t>Zambo Anguissa</t>
+          <t>Giovane</t>
         </is>
       </c>
       <c r="N31" t="inlineStr">
         <is>
-          <t>Bernede; Nelsson</t>
+          <t>Akpa Akpro; Gagliardini</t>
         </is>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>Di Lorenzo</t>
+          <t>Juan Jesus</t>
         </is>
       </c>
       <c r="P31" t="inlineStr"/>
@@ -2569,24 +2569,24 @@
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>Raspadori</t>
+          <t>Scamacca</t>
         </is>
       </c>
       <c r="K32" t="inlineStr"/>
       <c r="L32" t="inlineStr">
         <is>
-          <t>Scamacca</t>
+          <t>Raspadori</t>
         </is>
       </c>
       <c r="M32" t="inlineStr"/>
       <c r="N32" t="inlineStr">
         <is>
-          <t>Carnesecchi; De Ketelaere</t>
+          <t>Kolasinac; De Roon</t>
         </is>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>Karlstrom; Solet</t>
+          <t>Goglichidze *; Gueye</t>
         </is>
       </c>
       <c r="P32" t="inlineStr"/>
@@ -2640,18 +2640,18 @@
       <c r="K33" t="inlineStr"/>
       <c r="L33" t="inlineStr">
         <is>
-          <t>Orsolini</t>
+          <t>Dominguez B.</t>
         </is>
       </c>
       <c r="M33" t="inlineStr"/>
       <c r="N33" t="inlineStr">
         <is>
-          <t>Orsolini; Castro S.</t>
+          <t>De Silvestri; Lykogiannis</t>
         </is>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>Bernede; Nelsson</t>
+          <t>Akpa Akpro; Gagliardini</t>
         </is>
       </c>
       <c r="P33" t="inlineStr"/>
@@ -2700,23 +2700,23 @@
       <c r="J34" t="inlineStr"/>
       <c r="K34" t="inlineStr">
         <is>
-          <t>Baturina</t>
+          <t>Douvikas</t>
         </is>
       </c>
       <c r="L34" t="inlineStr"/>
       <c r="M34" t="inlineStr">
         <is>
-          <t>Paz N.</t>
+          <t>Baturina</t>
         </is>
       </c>
       <c r="N34" t="inlineStr">
         <is>
-          <t>Adopo; Caprile</t>
+          <t>Dossena; Obert</t>
         </is>
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>Butez; Paz N.</t>
+          <t>Smolcic I.; Diego Carlos</t>
         </is>
       </c>
       <c r="P34" t="inlineStr"/>
@@ -2764,24 +2764,24 @@
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>Brescianini</t>
+          <t>Kean</t>
         </is>
       </c>
       <c r="K35" t="inlineStr"/>
       <c r="L35" t="inlineStr">
         <is>
-          <t>Mandragora</t>
+          <t>Harrison</t>
         </is>
       </c>
       <c r="M35" t="inlineStr"/>
       <c r="N35" t="inlineStr">
         <is>
-          <t>De Gea; Dodò</t>
+          <t>Pongracic; Ranieri L.</t>
         </is>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>Bernabè; Pellegrino M.</t>
+          <t>Rinaldi; Nicolussi Caviglia</t>
         </is>
       </c>
       <c r="P35" t="inlineStr"/>
@@ -2830,23 +2830,23 @@
       <c r="J36" t="inlineStr"/>
       <c r="K36" t="inlineStr">
         <is>
-          <t>Soulè</t>
+          <t>Malen</t>
         </is>
       </c>
       <c r="L36" t="inlineStr"/>
       <c r="M36" t="inlineStr">
         <is>
-          <t>Malen</t>
+          <t>Zaragoza</t>
         </is>
       </c>
       <c r="N36" t="inlineStr">
         <is>
-          <t>Vasquez; Colombo</t>
+          <t>Gronbaek *; Malinovskyi</t>
         </is>
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>Svilar; Cristante</t>
+          <t>Zaragoza; Mancini</t>
         </is>
       </c>
       <c r="P36" t="inlineStr"/>
@@ -2894,24 +2894,24 @@
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>Yildiz; Bremer</t>
+          <t>Yildiz; Kostic</t>
         </is>
       </c>
       <c r="K37" t="inlineStr"/>
       <c r="L37" t="inlineStr">
         <is>
-          <t>Kostic; Adzic</t>
+          <t>Boga; Holm</t>
         </is>
       </c>
       <c r="M37" t="inlineStr"/>
       <c r="N37" t="inlineStr">
         <is>
-          <t>Kalulu</t>
+          <t>Gatti</t>
         </is>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>Canestrelli; Aebischer</t>
+          <t>Coppola F.; Denoon</t>
         </is>
       </c>
       <c r="P37" t="inlineStr"/>
@@ -2959,29 +2959,29 @@
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>Castellanos *</t>
+          <t>Pedro</t>
         </is>
       </c>
       <c r="K38" t="inlineStr"/>
       <c r="L38" t="inlineStr">
         <is>
-          <t>Isaksen</t>
+          <t>Castellanos *</t>
         </is>
       </c>
       <c r="M38" t="inlineStr"/>
       <c r="N38" t="inlineStr">
         <is>
-          <t>Provedel; Gila</t>
+          <t>Taylor K.; Zaccagni</t>
         </is>
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>Idzes; Laurientè</t>
+          <t>Iannoni; Thorstvedt</t>
         </is>
       </c>
       <c r="P38" t="inlineStr">
         <is>
-          <t>Basic</t>
+          <t>Belahyane</t>
         </is>
       </c>
       <c r="Q38" t="inlineStr"/>
@@ -3032,12 +3032,12 @@
       <c r="M39" t="inlineStr"/>
       <c r="N39" t="inlineStr">
         <is>
-          <t>Falcone; Gallo</t>
+          <t>Ramadani; Gaspar K.</t>
         </is>
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>Baschirotto; Terracciano F.</t>
+          <t>Pezzella Giu.; Payero</t>
         </is>
       </c>
       <c r="P39" t="inlineStr"/>
@@ -3095,7 +3095,7 @@
       </c>
       <c r="L40" t="inlineStr">
         <is>
-          <t>Leao</t>
+          <t>Rabiot</t>
         </is>
       </c>
       <c r="M40" t="inlineStr">
@@ -3105,12 +3105,12 @@
       </c>
       <c r="N40" t="inlineStr">
         <is>
-          <t>Maignan; Saelemaekers</t>
+          <t>Athekame; Estupinan</t>
         </is>
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>Martinez L.; Barella</t>
+          <t>Calhanoglu; Barella</t>
         </is>
       </c>
       <c r="P40" t="inlineStr"/>
@@ -3158,24 +3158,24 @@
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>De Bruyne; Zambo Anguissa</t>
+          <t>Santos A.; De Bruyne</t>
         </is>
       </c>
       <c r="K41" t="inlineStr"/>
       <c r="L41" t="inlineStr">
         <is>
-          <t>Vergara; McTominay</t>
+          <t>Giovane; Neres</t>
         </is>
       </c>
       <c r="M41" t="inlineStr"/>
       <c r="N41" t="inlineStr">
         <is>
-          <t>Di Lorenzo</t>
+          <t>Juan Jesus</t>
         </is>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>Lazaro; Vlasic</t>
+          <t>Aboukhlal; Nkounkou</t>
         </is>
       </c>
       <c r="P41" t="inlineStr"/>
@@ -3227,12 +3227,12 @@
       <c r="M42" t="inlineStr"/>
       <c r="N42" t="inlineStr">
         <is>
-          <t>Butez; Paz N.</t>
+          <t>Smolcic I.; Diego Carlos</t>
         </is>
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>Svilar; Cristante</t>
+          <t>Zaragoza; Mancini</t>
         </is>
       </c>
       <c r="P42" t="inlineStr"/>
@@ -3285,27 +3285,27 @@
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>Brescianini</t>
+          <t>Kean</t>
         </is>
       </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>Bonazzoli</t>
+          <t>Vandeputte</t>
         </is>
       </c>
       <c r="M43" t="inlineStr">
         <is>
-          <t>Mandragora</t>
+          <t>Harrison</t>
         </is>
       </c>
       <c r="N43" t="inlineStr">
         <is>
-          <t>Baschirotto; Terracciano F.</t>
+          <t>Pezzella Giu.; Payero</t>
         </is>
       </c>
       <c r="O43" t="inlineStr">
         <is>
-          <t>De Gea; Dodò</t>
+          <t>Pongracic; Ranieri L.</t>
         </is>
       </c>
       <c r="P43" t="inlineStr"/>
@@ -3365,12 +3365,12 @@
       <c r="M44" t="inlineStr"/>
       <c r="N44" t="inlineStr">
         <is>
-          <t>Martinez L.; Barella</t>
+          <t>Calhanoglu; Barella</t>
         </is>
       </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>Carnesecchi; De Ketelaere</t>
+          <t>Kolasinac; De Roon</t>
         </is>
       </c>
       <c r="P44" t="inlineStr"/>
@@ -3425,22 +3425,22 @@
       <c r="L45" t="inlineStr"/>
       <c r="M45" t="inlineStr">
         <is>
-          <t>Leao</t>
+          <t>Rabiot</t>
         </is>
       </c>
       <c r="N45" t="inlineStr">
         <is>
-          <t>Provedel; Gila</t>
+          <t>Taylor K.; Zaccagni</t>
         </is>
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>Maignan; Saelemaekers</t>
+          <t>Athekame; Estupinan</t>
         </is>
       </c>
       <c r="P45" t="inlineStr">
         <is>
-          <t>Basic</t>
+          <t>Belahyane</t>
         </is>
       </c>
       <c r="Q45" t="inlineStr"/>
@@ -3487,24 +3487,24 @@
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>De Bruyne</t>
+          <t>Santos A.</t>
         </is>
       </c>
       <c r="K46" t="inlineStr"/>
       <c r="L46" t="inlineStr">
         <is>
-          <t>Zambo Anguissa</t>
+          <t>Giovane</t>
         </is>
       </c>
       <c r="M46" t="inlineStr"/>
       <c r="N46" t="inlineStr">
         <is>
-          <t>Di Lorenzo</t>
+          <t>Juan Jesus</t>
         </is>
       </c>
       <c r="O46" t="inlineStr">
         <is>
-          <t>Falcone; Gallo</t>
+          <t>Ramadani; Gaspar K.</t>
         </is>
       </c>
       <c r="P46" t="inlineStr"/>
@@ -3559,17 +3559,17 @@
       <c r="L47" t="inlineStr"/>
       <c r="M47" t="inlineStr">
         <is>
-          <t>Kilicsoy</t>
+          <t>Mazzitelli</t>
         </is>
       </c>
       <c r="N47" t="inlineStr">
         <is>
-          <t>Canestrelli; Aebischer</t>
+          <t>Coppola F.; Denoon</t>
         </is>
       </c>
       <c r="O47" t="inlineStr">
         <is>
-          <t>Adopo; Caprile</t>
+          <t>Dossena; Obert</t>
         </is>
       </c>
       <c r="P47" t="inlineStr"/>
@@ -3627,22 +3627,22 @@
       </c>
       <c r="L48" t="inlineStr">
         <is>
-          <t>Volpato</t>
+          <t>Garcia U.</t>
         </is>
       </c>
       <c r="M48" t="inlineStr">
         <is>
-          <t>Orsolini</t>
+          <t>Dominguez B.</t>
         </is>
       </c>
       <c r="N48" t="inlineStr">
         <is>
-          <t>Idzes; Laurientè</t>
+          <t>Iannoni; Thorstvedt</t>
         </is>
       </c>
       <c r="O48" t="inlineStr">
         <is>
-          <t>Orsolini; Castro S.</t>
+          <t>De Silvestri; Lykogiannis</t>
         </is>
       </c>
       <c r="P48" t="inlineStr"/>
@@ -3702,12 +3702,12 @@
       <c r="M49" t="inlineStr"/>
       <c r="N49" t="inlineStr">
         <is>
-          <t>Lazaro; Vlasic</t>
+          <t>Aboukhlal; Nkounkou</t>
         </is>
       </c>
       <c r="O49" t="inlineStr">
         <is>
-          <t>Bernabè; Pellegrino M.</t>
+          <t>Rinaldi; Nicolussi Caviglia</t>
         </is>
       </c>
       <c r="P49" t="inlineStr"/>
@@ -3756,23 +3756,23 @@
       <c r="J50" t="inlineStr"/>
       <c r="K50" t="inlineStr">
         <is>
-          <t>Yildiz; Bremer</t>
+          <t>Yildiz; Kostic</t>
         </is>
       </c>
       <c r="L50" t="inlineStr"/>
       <c r="M50" t="inlineStr">
         <is>
-          <t>Kostic; Adzic</t>
+          <t>Boga; Holm</t>
         </is>
       </c>
       <c r="N50" t="inlineStr">
         <is>
-          <t>Karlstrom; Solet</t>
+          <t>Goglichidze *; Gueye</t>
         </is>
       </c>
       <c r="O50" t="inlineStr">
         <is>
-          <t>Kalulu</t>
+          <t>Gatti</t>
         </is>
       </c>
       <c r="P50" t="inlineStr"/>
@@ -3820,32 +3820,32 @@
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>Edmundsson</t>
+          <t>Orban G.</t>
         </is>
       </c>
       <c r="K51" t="inlineStr">
         <is>
-          <t>Malinovskyi</t>
+          <t>Colombo</t>
         </is>
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>Orban G.</t>
+          <t>Lovric</t>
         </is>
       </c>
       <c r="M51" t="inlineStr">
         <is>
-          <t>Ostigard</t>
+          <t>Martin</t>
         </is>
       </c>
       <c r="N51" t="inlineStr">
         <is>
-          <t>Bernede; Nelsson</t>
+          <t>Akpa Akpro; Gagliardini</t>
         </is>
       </c>
       <c r="O51" t="inlineStr">
         <is>
-          <t>Vasquez; Colombo</t>
+          <t>Gronbaek *; Malinovskyi</t>
         </is>
       </c>
       <c r="P51" t="inlineStr"/>
@@ -3893,24 +3893,24 @@
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>Raspadori</t>
+          <t>Scamacca</t>
         </is>
       </c>
       <c r="K52" t="inlineStr"/>
       <c r="L52" t="inlineStr">
         <is>
-          <t>Scamacca</t>
+          <t>Raspadori</t>
         </is>
       </c>
       <c r="M52" t="inlineStr"/>
       <c r="N52" t="inlineStr">
         <is>
-          <t>Carnesecchi; De Ketelaere</t>
+          <t>Kolasinac; De Roon</t>
         </is>
       </c>
       <c r="O52" t="inlineStr">
         <is>
-          <t>Bernede; Nelsson</t>
+          <t>Akpa Akpro; Gagliardini</t>
         </is>
       </c>
       <c r="P52" t="inlineStr"/>
@@ -3963,33 +3963,33 @@
       </c>
       <c r="K53" t="inlineStr">
         <is>
+          <t>Pedro</t>
+        </is>
+      </c>
+      <c r="L53" t="inlineStr">
+        <is>
+          <t>Dominguez B.</t>
+        </is>
+      </c>
+      <c r="M53" t="inlineStr">
+        <is>
           <t>Castellanos *</t>
         </is>
       </c>
-      <c r="L53" t="inlineStr">
-        <is>
-          <t>Orsolini</t>
-        </is>
-      </c>
-      <c r="M53" t="inlineStr">
-        <is>
-          <t>Isaksen</t>
-        </is>
-      </c>
       <c r="N53" t="inlineStr">
         <is>
-          <t>Orsolini; Castro S.</t>
+          <t>De Silvestri; Lykogiannis</t>
         </is>
       </c>
       <c r="O53" t="inlineStr">
         <is>
-          <t>Provedel; Gila</t>
+          <t>Taylor K.; Zaccagni</t>
         </is>
       </c>
       <c r="P53" t="inlineStr"/>
       <c r="Q53" t="inlineStr">
         <is>
-          <t>Basic</t>
+          <t>Belahyane</t>
         </is>
       </c>
       <c r="R53" t="n">
@@ -4036,23 +4036,23 @@
       <c r="J54" t="inlineStr"/>
       <c r="K54" t="inlineStr">
         <is>
-          <t>De Bruyne</t>
+          <t>Santos A.</t>
         </is>
       </c>
       <c r="L54" t="inlineStr"/>
       <c r="M54" t="inlineStr">
         <is>
-          <t>Zambo Anguissa</t>
+          <t>Giovane</t>
         </is>
       </c>
       <c r="N54" t="inlineStr">
         <is>
-          <t>Adopo; Caprile</t>
+          <t>Dossena; Obert</t>
         </is>
       </c>
       <c r="O54" t="inlineStr">
         <is>
-          <t>Di Lorenzo</t>
+          <t>Juan Jesus</t>
         </is>
       </c>
       <c r="P54" t="inlineStr"/>
@@ -4100,24 +4100,24 @@
       </c>
       <c r="J55" t="inlineStr">
         <is>
-          <t>Baturina; Paz N.</t>
+          <t>Douvikas; Baturina</t>
         </is>
       </c>
       <c r="K55" t="inlineStr"/>
       <c r="L55" t="inlineStr">
         <is>
-          <t>Douvikas; Kempf</t>
+          <t>Rodriguez Je.; Paz N.</t>
         </is>
       </c>
       <c r="M55" t="inlineStr"/>
       <c r="N55" t="inlineStr">
         <is>
-          <t>Butez; Paz N.</t>
+          <t>Smolcic I.; Diego Carlos</t>
         </is>
       </c>
       <c r="O55" t="inlineStr">
         <is>
-          <t>Canestrelli; Aebischer</t>
+          <t>Coppola F.; Denoon</t>
         </is>
       </c>
       <c r="P55" t="inlineStr"/>
@@ -4166,23 +4166,23 @@
       <c r="J56" t="inlineStr"/>
       <c r="K56" t="inlineStr">
         <is>
-          <t>Martinez L.; Dimarco</t>
+          <t>Martinez L.; Calhanoglu</t>
         </is>
       </c>
       <c r="L56" t="inlineStr"/>
       <c r="M56" t="inlineStr">
         <is>
-          <t>Calhanoglu; Bonny</t>
+          <t>Dimarco; Barella</t>
         </is>
       </c>
       <c r="N56" t="inlineStr">
         <is>
-          <t>De Gea; Dodò</t>
+          <t>Pongracic; Ranieri L.</t>
         </is>
       </c>
       <c r="O56" t="inlineStr">
         <is>
-          <t>Martinez L.; Barella</t>
+          <t>Calhanoglu; Barella</t>
         </is>
       </c>
       <c r="P56" t="inlineStr"/>
@@ -4230,7 +4230,7 @@
       </c>
       <c r="J57" t="inlineStr">
         <is>
-          <t>Malinovskyi</t>
+          <t>Colombo</t>
         </is>
       </c>
       <c r="K57" t="inlineStr">
@@ -4240,22 +4240,22 @@
       </c>
       <c r="L57" t="inlineStr">
         <is>
-          <t>Ostigard</t>
+          <t>Martin</t>
         </is>
       </c>
       <c r="M57" t="inlineStr">
         <is>
-          <t>Zaniolo</t>
+          <t>Rui Modesto *</t>
         </is>
       </c>
       <c r="N57" t="inlineStr">
         <is>
-          <t>Vasquez; Colombo</t>
+          <t>Gronbaek *; Malinovskyi</t>
         </is>
       </c>
       <c r="O57" t="inlineStr">
         <is>
-          <t>Karlstrom; Solet</t>
+          <t>Goglichidze *; Gueye</t>
         </is>
       </c>
       <c r="P57" t="inlineStr"/>
@@ -4303,24 +4303,24 @@
       </c>
       <c r="J58" t="inlineStr">
         <is>
-          <t>Yildiz; Bremer</t>
+          <t>Yildiz; Kostic</t>
         </is>
       </c>
       <c r="K58" t="inlineStr"/>
       <c r="L58" t="inlineStr">
         <is>
-          <t>Kostic; Adzic</t>
+          <t>Boga; Holm</t>
         </is>
       </c>
       <c r="M58" t="inlineStr"/>
       <c r="N58" t="inlineStr">
         <is>
-          <t>Kalulu</t>
+          <t>Gatti</t>
         </is>
       </c>
       <c r="O58" t="inlineStr">
         <is>
-          <t>Idzes; Laurientè</t>
+          <t>Iannoni; Thorstvedt</t>
         </is>
       </c>
       <c r="P58" t="inlineStr"/>
@@ -4374,18 +4374,18 @@
       <c r="K59" t="inlineStr"/>
       <c r="L59" t="inlineStr">
         <is>
-          <t>Rabiot; Nkunku</t>
+          <t>Rabiot; Athekame</t>
         </is>
       </c>
       <c r="M59" t="inlineStr"/>
       <c r="N59" t="inlineStr">
         <is>
-          <t>Maignan; Saelemaekers</t>
+          <t>Athekame; Estupinan</t>
         </is>
       </c>
       <c r="O59" t="inlineStr">
         <is>
-          <t>Lazaro; Vlasic</t>
+          <t>Aboukhlal; Nkounkou</t>
         </is>
       </c>
       <c r="P59" t="inlineStr"/>
@@ -4437,12 +4437,12 @@
       <c r="M60" t="inlineStr"/>
       <c r="N60" t="inlineStr">
         <is>
-          <t>Bernabè; Pellegrino M.</t>
+          <t>Rinaldi; Nicolussi Caviglia</t>
         </is>
       </c>
       <c r="O60" t="inlineStr">
         <is>
-          <t>Baschirotto; Terracciano F.</t>
+          <t>Pezzella Giu.; Payero</t>
         </is>
       </c>
       <c r="P60" t="inlineStr"/>
@@ -4490,24 +4490,24 @@
       </c>
       <c r="J61" t="inlineStr">
         <is>
-          <t>Soulè</t>
+          <t>Malen</t>
         </is>
       </c>
       <c r="K61" t="inlineStr"/>
       <c r="L61" t="inlineStr">
         <is>
-          <t>Malen</t>
+          <t>Zaragoza</t>
         </is>
       </c>
       <c r="M61" t="inlineStr"/>
       <c r="N61" t="inlineStr">
         <is>
-          <t>Svilar; Cristante</t>
+          <t>Zaragoza; Mancini</t>
         </is>
       </c>
       <c r="O61" t="inlineStr">
         <is>
-          <t>Falcone; Gallo</t>
+          <t>Ramadani; Gaspar K.</t>
         </is>
       </c>
       <c r="P61" t="inlineStr"/>
@@ -4565,22 +4565,22 @@
       </c>
       <c r="L62" t="inlineStr">
         <is>
-          <t>Bonazzoli</t>
+          <t>Vandeputte</t>
         </is>
       </c>
       <c r="M62" t="inlineStr">
         <is>
-          <t>Orsolini</t>
+          <t>Dominguez B.</t>
         </is>
       </c>
       <c r="N62" t="inlineStr">
         <is>
-          <t>Baschirotto; Terracciano F.</t>
+          <t>Pezzella Giu.; Payero</t>
         </is>
       </c>
       <c r="O62" t="inlineStr">
         <is>
-          <t>Orsolini; Castro S.</t>
+          <t>De Silvestri; Lykogiannis</t>
         </is>
       </c>
       <c r="P62" t="inlineStr"/>
@@ -4640,12 +4640,12 @@
       <c r="M63" t="inlineStr"/>
       <c r="N63" t="inlineStr">
         <is>
-          <t>Martinez L.; Barella</t>
+          <t>Calhanoglu; Barella</t>
         </is>
       </c>
       <c r="O63" t="inlineStr">
         <is>
-          <t>Svilar; Cristante</t>
+          <t>Zaragoza; Mancini</t>
         </is>
       </c>
       <c r="P63" t="inlineStr"/>
@@ -4693,24 +4693,24 @@
       </c>
       <c r="J64" t="inlineStr">
         <is>
-          <t>Yildiz; Bremer</t>
+          <t>Yildiz; Kostic</t>
         </is>
       </c>
       <c r="K64" t="inlineStr"/>
       <c r="L64" t="inlineStr">
         <is>
-          <t>Kostic; Adzic</t>
+          <t>Boga; Holm</t>
         </is>
       </c>
       <c r="M64" t="inlineStr"/>
       <c r="N64" t="inlineStr">
         <is>
-          <t>Kalulu</t>
+          <t>Gatti</t>
         </is>
       </c>
       <c r="O64" t="inlineStr">
         <is>
-          <t>Vasquez; Colombo</t>
+          <t>Gronbaek *; Malinovskyi</t>
         </is>
       </c>
       <c r="P64" t="inlineStr"/>
@@ -4758,29 +4758,29 @@
       </c>
       <c r="J65" t="inlineStr">
         <is>
-          <t>Castellanos *</t>
+          <t>Pedro</t>
         </is>
       </c>
       <c r="K65" t="inlineStr"/>
       <c r="L65" t="inlineStr">
         <is>
-          <t>Isaksen</t>
+          <t>Castellanos *</t>
         </is>
       </c>
       <c r="M65" t="inlineStr"/>
       <c r="N65" t="inlineStr">
         <is>
-          <t>Provedel; Gila</t>
+          <t>Taylor K.; Zaccagni</t>
         </is>
       </c>
       <c r="O65" t="inlineStr">
         <is>
-          <t>Bernabè; Pellegrino M.</t>
+          <t>Rinaldi; Nicolussi Caviglia</t>
         </is>
       </c>
       <c r="P65" t="inlineStr">
         <is>
-          <t>Basic</t>
+          <t>Belahyane</t>
         </is>
       </c>
       <c r="Q65" t="inlineStr"/>
@@ -4828,23 +4828,23 @@
       <c r="J66" t="inlineStr"/>
       <c r="K66" t="inlineStr">
         <is>
-          <t>Raspadori</t>
+          <t>Scamacca</t>
         </is>
       </c>
       <c r="L66" t="inlineStr"/>
       <c r="M66" t="inlineStr">
         <is>
-          <t>Scamacca</t>
+          <t>Raspadori</t>
         </is>
       </c>
       <c r="N66" t="inlineStr">
         <is>
-          <t>Falcone; Gallo</t>
+          <t>Ramadani; Gaspar K.</t>
         </is>
       </c>
       <c r="O66" t="inlineStr">
         <is>
-          <t>Carnesecchi; De Ketelaere</t>
+          <t>Kolasinac; De Roon</t>
         </is>
       </c>
       <c r="P66" t="inlineStr"/>
@@ -4899,17 +4899,17 @@
       <c r="L67" t="inlineStr"/>
       <c r="M67" t="inlineStr">
         <is>
-          <t>Leao</t>
+          <t>Rabiot</t>
         </is>
       </c>
       <c r="N67" t="inlineStr">
         <is>
-          <t>Di Lorenzo</t>
+          <t>Juan Jesus</t>
         </is>
       </c>
       <c r="O67" t="inlineStr">
         <is>
-          <t>Maignan; Saelemaekers</t>
+          <t>Athekame; Estupinan</t>
         </is>
       </c>
       <c r="P67" t="inlineStr"/>
@@ -4957,19 +4957,19 @@
       </c>
       <c r="J68" t="inlineStr">
         <is>
+          <t>Loyola</t>
+        </is>
+      </c>
+      <c r="K68" t="inlineStr">
+        <is>
+          <t>Simeone</t>
+        </is>
+      </c>
+      <c r="L68" t="inlineStr">
+        <is>
           <t>Durosinmi</t>
         </is>
       </c>
-      <c r="K68" t="inlineStr">
-        <is>
-          <t>Simeone</t>
-        </is>
-      </c>
-      <c r="L68" t="inlineStr">
-        <is>
-          <t>Moreo</t>
-        </is>
-      </c>
       <c r="M68" t="inlineStr">
         <is>
           <t>Njie</t>
@@ -4977,12 +4977,12 @@
       </c>
       <c r="N68" t="inlineStr">
         <is>
-          <t>Canestrelli; Aebischer</t>
+          <t>Coppola F.; Denoon</t>
         </is>
       </c>
       <c r="O68" t="inlineStr">
         <is>
-          <t>Lazaro; Vlasic</t>
+          <t>Aboukhlal; Nkounkou</t>
         </is>
       </c>
       <c r="P68" t="inlineStr"/>
@@ -5040,22 +5040,22 @@
       </c>
       <c r="L69" t="inlineStr">
         <is>
-          <t>Volpato</t>
+          <t>Garcia U.</t>
         </is>
       </c>
       <c r="M69" t="inlineStr">
         <is>
-          <t>Kilicsoy</t>
+          <t>Mazzitelli</t>
         </is>
       </c>
       <c r="N69" t="inlineStr">
         <is>
-          <t>Idzes; Laurientè</t>
+          <t>Iannoni; Thorstvedt</t>
         </is>
       </c>
       <c r="O69" t="inlineStr">
         <is>
-          <t>Adopo; Caprile</t>
+          <t>Dossena; Obert</t>
         </is>
       </c>
       <c r="P69" t="inlineStr"/>
@@ -5104,23 +5104,23 @@
       <c r="J70" t="inlineStr"/>
       <c r="K70" t="inlineStr">
         <is>
-          <t>Baturina</t>
+          <t>Douvikas</t>
         </is>
       </c>
       <c r="L70" t="inlineStr"/>
       <c r="M70" t="inlineStr">
         <is>
-          <t>Paz N.</t>
+          <t>Baturina</t>
         </is>
       </c>
       <c r="N70" t="inlineStr">
         <is>
-          <t>Karlstrom; Solet</t>
+          <t>Goglichidze *; Gueye</t>
         </is>
       </c>
       <c r="O70" t="inlineStr">
         <is>
-          <t>Butez; Paz N.</t>
+          <t>Smolcic I.; Diego Carlos</t>
         </is>
       </c>
       <c r="P70" t="inlineStr"/>
@@ -5168,32 +5168,32 @@
       </c>
       <c r="J71" t="inlineStr">
         <is>
-          <t>Edmundsson</t>
+          <t>Orban G.</t>
         </is>
       </c>
       <c r="K71" t="inlineStr">
         <is>
-          <t>Brescianini</t>
+          <t>Kean</t>
         </is>
       </c>
       <c r="L71" t="inlineStr">
         <is>
-          <t>Orban G.</t>
+          <t>Lovric</t>
         </is>
       </c>
       <c r="M71" t="inlineStr">
         <is>
-          <t>Mandragora</t>
+          <t>Harrison</t>
         </is>
       </c>
       <c r="N71" t="inlineStr">
         <is>
-          <t>Bernede; Nelsson</t>
+          <t>Akpa Akpro; Gagliardini</t>
         </is>
       </c>
       <c r="O71" t="inlineStr">
         <is>
-          <t>De Gea; Dodò</t>
+          <t>Pongracic; Ranieri L.</t>
         </is>
       </c>
       <c r="P71" t="inlineStr"/>
@@ -5248,17 +5248,17 @@
       <c r="L72" t="inlineStr"/>
       <c r="M72" t="inlineStr">
         <is>
-          <t>Bremer</t>
+          <t>Boga</t>
         </is>
       </c>
       <c r="N72" t="inlineStr">
         <is>
-          <t>Carnesecchi; De Ketelaere</t>
+          <t>Kolasinac; De Roon</t>
         </is>
       </c>
       <c r="O72" t="inlineStr">
         <is>
-          <t>Kalulu</t>
+          <t>Gatti</t>
         </is>
       </c>
       <c r="P72" t="inlineStr"/>
@@ -5312,18 +5312,18 @@
       <c r="K73" t="inlineStr"/>
       <c r="L73" t="inlineStr">
         <is>
-          <t>Orsolini</t>
+          <t>Dominguez B.</t>
         </is>
       </c>
       <c r="M73" t="inlineStr"/>
       <c r="N73" t="inlineStr">
         <is>
-          <t>Orsolini; Castro S.</t>
+          <t>De Silvestri; Lykogiannis</t>
         </is>
       </c>
       <c r="O73" t="inlineStr">
         <is>
-          <t>Falcone; Gallo</t>
+          <t>Ramadani; Gaspar K.</t>
         </is>
       </c>
       <c r="P73" t="inlineStr"/>
@@ -5377,18 +5377,18 @@
       <c r="K74" t="inlineStr"/>
       <c r="L74" t="inlineStr">
         <is>
-          <t>Kilicsoy</t>
+          <t>Mazzitelli</t>
         </is>
       </c>
       <c r="M74" t="inlineStr"/>
       <c r="N74" t="inlineStr">
         <is>
-          <t>Adopo; Caprile</t>
+          <t>Dossena; Obert</t>
         </is>
       </c>
       <c r="O74" t="inlineStr">
         <is>
-          <t>Baschirotto; Terracciano F.</t>
+          <t>Pezzella Giu.; Payero</t>
         </is>
       </c>
       <c r="P74" t="inlineStr"/>
@@ -5436,19 +5436,19 @@
       </c>
       <c r="J75" t="inlineStr">
         <is>
+          <t>Douvikas</t>
+        </is>
+      </c>
+      <c r="K75" t="inlineStr">
+        <is>
+          <t>Martinez L.</t>
+        </is>
+      </c>
+      <c r="L75" t="inlineStr">
+        <is>
           <t>Baturina</t>
         </is>
       </c>
-      <c r="K75" t="inlineStr">
-        <is>
-          <t>Martinez L.</t>
-        </is>
-      </c>
-      <c r="L75" t="inlineStr">
-        <is>
-          <t>Paz N.</t>
-        </is>
-      </c>
       <c r="M75" t="inlineStr">
         <is>
           <t>Dimarco</t>
@@ -5456,12 +5456,12 @@
       </c>
       <c r="N75" t="inlineStr">
         <is>
-          <t>Butez; Paz N.</t>
+          <t>Smolcic I.; Diego Carlos</t>
         </is>
       </c>
       <c r="O75" t="inlineStr">
         <is>
-          <t>Martinez L.; Barella</t>
+          <t>Calhanoglu; Barella</t>
         </is>
       </c>
       <c r="P75" t="inlineStr"/>
@@ -5510,29 +5510,29 @@
       <c r="J76" t="inlineStr"/>
       <c r="K76" t="inlineStr">
         <is>
-          <t>Castellanos *</t>
+          <t>Pedro</t>
         </is>
       </c>
       <c r="L76" t="inlineStr"/>
       <c r="M76" t="inlineStr">
         <is>
-          <t>Isaksen</t>
+          <t>Castellanos *</t>
         </is>
       </c>
       <c r="N76" t="inlineStr">
         <is>
-          <t>De Gea; Dodò</t>
+          <t>Pongracic; Ranieri L.</t>
         </is>
       </c>
       <c r="O76" t="inlineStr">
         <is>
-          <t>Provedel; Gila</t>
+          <t>Taylor K.; Zaccagni</t>
         </is>
       </c>
       <c r="P76" t="inlineStr"/>
       <c r="Q76" t="inlineStr">
         <is>
-          <t>Basic</t>
+          <t>Belahyane</t>
         </is>
       </c>
       <c r="R76" t="n">
@@ -5578,7 +5578,7 @@
       </c>
       <c r="J77" t="inlineStr">
         <is>
-          <t>Malinovskyi</t>
+          <t>Colombo</t>
         </is>
       </c>
       <c r="K77" t="inlineStr">
@@ -5588,22 +5588,22 @@
       </c>
       <c r="L77" t="inlineStr">
         <is>
-          <t>Ostigard</t>
+          <t>Martin</t>
         </is>
       </c>
       <c r="M77" t="inlineStr">
         <is>
-          <t>Volpato</t>
+          <t>Garcia U.</t>
         </is>
       </c>
       <c r="N77" t="inlineStr">
         <is>
-          <t>Vasquez; Colombo</t>
+          <t>Gronbaek *; Malinovskyi</t>
         </is>
       </c>
       <c r="O77" t="inlineStr">
         <is>
-          <t>Idzes; Laurientè</t>
+          <t>Iannoni; Thorstvedt</t>
         </is>
       </c>
       <c r="P77" t="inlineStr"/>
@@ -5657,18 +5657,18 @@
       <c r="K78" t="inlineStr"/>
       <c r="L78" t="inlineStr">
         <is>
-          <t>Rabiot; Nkunku</t>
+          <t>Rabiot; Athekame</t>
         </is>
       </c>
       <c r="M78" t="inlineStr"/>
       <c r="N78" t="inlineStr">
         <is>
-          <t>Maignan; Saelemaekers</t>
+          <t>Athekame; Estupinan</t>
         </is>
       </c>
       <c r="O78" t="inlineStr">
         <is>
-          <t>Karlstrom; Solet</t>
+          <t>Goglichidze *; Gueye</t>
         </is>
       </c>
       <c r="P78" t="inlineStr"/>
@@ -5717,23 +5717,23 @@
       <c r="J79" t="inlineStr"/>
       <c r="K79" t="inlineStr">
         <is>
-          <t>De Bruyne</t>
+          <t>Santos A.</t>
         </is>
       </c>
       <c r="L79" t="inlineStr"/>
       <c r="M79" t="inlineStr">
         <is>
-          <t>Zambo Anguissa</t>
+          <t>Giovane</t>
         </is>
       </c>
       <c r="N79" t="inlineStr">
         <is>
-          <t>Bernabè; Pellegrino M.</t>
+          <t>Rinaldi; Nicolussi Caviglia</t>
         </is>
       </c>
       <c r="O79" t="inlineStr">
         <is>
-          <t>Di Lorenzo</t>
+          <t>Juan Jesus</t>
         </is>
       </c>
       <c r="P79" t="inlineStr"/>
@@ -5781,24 +5781,24 @@
       </c>
       <c r="J80" t="inlineStr">
         <is>
-          <t>Soulè</t>
+          <t>Malen</t>
         </is>
       </c>
       <c r="K80" t="inlineStr"/>
       <c r="L80" t="inlineStr">
         <is>
-          <t>Malen</t>
+          <t>Zaragoza</t>
         </is>
       </c>
       <c r="M80" t="inlineStr"/>
       <c r="N80" t="inlineStr">
         <is>
-          <t>Svilar; Cristante</t>
+          <t>Zaragoza; Mancini</t>
         </is>
       </c>
       <c r="O80" t="inlineStr">
         <is>
-          <t>Canestrelli; Aebischer</t>
+          <t>Coppola F.; Denoon</t>
         </is>
       </c>
       <c r="P80" t="inlineStr"/>
@@ -5851,7 +5851,7 @@
       </c>
       <c r="K81" t="inlineStr">
         <is>
-          <t>Edmundsson</t>
+          <t>Orban G.</t>
         </is>
       </c>
       <c r="L81" t="inlineStr">
@@ -5861,17 +5861,17 @@
       </c>
       <c r="M81" t="inlineStr">
         <is>
-          <t>Orban G.</t>
+          <t>Lovric</t>
         </is>
       </c>
       <c r="N81" t="inlineStr">
         <is>
-          <t>Lazaro; Vlasic</t>
+          <t>Aboukhlal; Nkounkou</t>
         </is>
       </c>
       <c r="O81" t="inlineStr">
         <is>
-          <t>Bernede; Nelsson</t>
+          <t>Akpa Akpro; Gagliardini</t>
         </is>
       </c>
       <c r="P81" t="inlineStr"/>
@@ -5929,7 +5929,7 @@
       </c>
       <c r="L82" t="inlineStr">
         <is>
-          <t>Bonazzoli</t>
+          <t>Vandeputte</t>
         </is>
       </c>
       <c r="M82" t="inlineStr">
@@ -5939,12 +5939,12 @@
       </c>
       <c r="N82" t="inlineStr">
         <is>
-          <t>Baschirotto; Terracciano F.</t>
+          <t>Pezzella Giu.; Payero</t>
         </is>
       </c>
       <c r="O82" t="inlineStr">
         <is>
-          <t>Lazaro; Vlasic</t>
+          <t>Aboukhlal; Nkounkou</t>
         </is>
       </c>
       <c r="P82" t="inlineStr"/>
@@ -5992,24 +5992,24 @@
       </c>
       <c r="J83" t="inlineStr">
         <is>
-          <t>Martinez L.; Dimarco</t>
+          <t>Martinez L.; Calhanoglu</t>
         </is>
       </c>
       <c r="K83" t="inlineStr"/>
       <c r="L83" t="inlineStr">
         <is>
-          <t>Calhanoglu; Bonny</t>
+          <t>Dimarco; Barella</t>
         </is>
       </c>
       <c r="M83" t="inlineStr"/>
       <c r="N83" t="inlineStr">
         <is>
-          <t>Martinez L.; Barella</t>
+          <t>Calhanoglu; Barella</t>
         </is>
       </c>
       <c r="O83" t="inlineStr">
         <is>
-          <t>Adopo; Caprile</t>
+          <t>Dossena; Obert</t>
         </is>
       </c>
       <c r="P83" t="inlineStr"/>
@@ -6063,18 +6063,18 @@
       <c r="K84" t="inlineStr"/>
       <c r="L84" t="inlineStr">
         <is>
-          <t>Bremer</t>
+          <t>Boga</t>
         </is>
       </c>
       <c r="M84" t="inlineStr"/>
       <c r="N84" t="inlineStr">
         <is>
-          <t>Kalulu</t>
+          <t>Gatti</t>
         </is>
       </c>
       <c r="O84" t="inlineStr">
         <is>
-          <t>Orsolini; Castro S.</t>
+          <t>De Silvestri; Lykogiannis</t>
         </is>
       </c>
       <c r="P84" t="inlineStr"/>
@@ -6123,23 +6123,23 @@
       <c r="J85" t="inlineStr"/>
       <c r="K85" t="inlineStr">
         <is>
-          <t>Brescianini</t>
+          <t>Kean</t>
         </is>
       </c>
       <c r="L85" t="inlineStr"/>
       <c r="M85" t="inlineStr">
         <is>
-          <t>Mandragora</t>
+          <t>Harrison</t>
         </is>
       </c>
       <c r="N85" t="inlineStr">
         <is>
-          <t>Falcone; Gallo</t>
+          <t>Ramadani; Gaspar K.</t>
         </is>
       </c>
       <c r="O85" t="inlineStr">
         <is>
-          <t>De Gea; Dodò</t>
+          <t>Pongracic; Ranieri L.</t>
         </is>
       </c>
       <c r="P85" t="inlineStr"/>
@@ -6187,30 +6187,30 @@
       </c>
       <c r="J86" t="inlineStr">
         <is>
-          <t>De Bruyne</t>
+          <t>Santos A.</t>
         </is>
       </c>
       <c r="K86" t="inlineStr"/>
       <c r="L86" t="inlineStr">
         <is>
-          <t>Zambo Anguissa</t>
+          <t>Giovane</t>
         </is>
       </c>
       <c r="M86" t="inlineStr"/>
       <c r="N86" t="inlineStr">
         <is>
-          <t>Di Lorenzo</t>
+          <t>Juan Jesus</t>
         </is>
       </c>
       <c r="O86" t="inlineStr">
         <is>
-          <t>Provedel; Gila</t>
+          <t>Taylor K.; Zaccagni</t>
         </is>
       </c>
       <c r="P86" t="inlineStr"/>
       <c r="Q86" t="inlineStr">
         <is>
-          <t>Basic</t>
+          <t>Belahyane</t>
         </is>
       </c>
       <c r="R86" t="n">
@@ -6256,32 +6256,32 @@
       </c>
       <c r="J87" t="inlineStr">
         <is>
+          <t>Loyola</t>
+        </is>
+      </c>
+      <c r="K87" t="inlineStr">
+        <is>
+          <t>Colombo</t>
+        </is>
+      </c>
+      <c r="L87" t="inlineStr">
+        <is>
           <t>Durosinmi</t>
         </is>
       </c>
-      <c r="K87" t="inlineStr">
-        <is>
-          <t>Malinovskyi</t>
-        </is>
-      </c>
-      <c r="L87" t="inlineStr">
-        <is>
-          <t>Moreo</t>
-        </is>
-      </c>
       <c r="M87" t="inlineStr">
         <is>
-          <t>Ostigard</t>
+          <t>Martin</t>
         </is>
       </c>
       <c r="N87" t="inlineStr">
         <is>
-          <t>Canestrelli; Aebischer</t>
+          <t>Coppola F.; Denoon</t>
         </is>
       </c>
       <c r="O87" t="inlineStr">
         <is>
-          <t>Vasquez; Colombo</t>
+          <t>Gronbaek *; Malinovskyi</t>
         </is>
       </c>
       <c r="P87" t="inlineStr"/>
@@ -6333,12 +6333,12 @@
       <c r="M88" t="inlineStr"/>
       <c r="N88" t="inlineStr">
         <is>
-          <t>Svilar; Cristante</t>
+          <t>Zaragoza; Mancini</t>
         </is>
       </c>
       <c r="O88" t="inlineStr">
         <is>
-          <t>Carnesecchi; De Ketelaere</t>
+          <t>Kolasinac; De Roon</t>
         </is>
       </c>
       <c r="P88" t="inlineStr"/>
@@ -6387,23 +6387,23 @@
       <c r="J89" t="inlineStr"/>
       <c r="K89" t="inlineStr">
         <is>
-          <t>Baturina</t>
+          <t>Douvikas</t>
         </is>
       </c>
       <c r="L89" t="inlineStr"/>
       <c r="M89" t="inlineStr">
         <is>
-          <t>Paz N.</t>
+          <t>Baturina</t>
         </is>
       </c>
       <c r="N89" t="inlineStr">
         <is>
-          <t>Idzes; Laurientè</t>
+          <t>Iannoni; Thorstvedt</t>
         </is>
       </c>
       <c r="O89" t="inlineStr">
         <is>
-          <t>Butez; Paz N.</t>
+          <t>Smolcic I.; Diego Carlos</t>
         </is>
       </c>
       <c r="P89" t="inlineStr"/>
@@ -6457,18 +6457,18 @@
       <c r="K90" t="inlineStr"/>
       <c r="L90" t="inlineStr">
         <is>
-          <t>Zaniolo</t>
+          <t>Rui Modesto *</t>
         </is>
       </c>
       <c r="M90" t="inlineStr"/>
       <c r="N90" t="inlineStr">
         <is>
-          <t>Karlstrom; Solet</t>
+          <t>Goglichidze *; Gueye</t>
         </is>
       </c>
       <c r="O90" t="inlineStr">
         <is>
-          <t>Bernabè; Pellegrino M.</t>
+          <t>Rinaldi; Nicolussi Caviglia</t>
         </is>
       </c>
       <c r="P90" t="inlineStr"/>
@@ -6523,17 +6523,17 @@
       <c r="L91" t="inlineStr"/>
       <c r="M91" t="inlineStr">
         <is>
-          <t>Rabiot; Nkunku</t>
+          <t>Rabiot; Athekame</t>
         </is>
       </c>
       <c r="N91" t="inlineStr">
         <is>
-          <t>Bernede; Nelsson</t>
+          <t>Akpa Akpro; Gagliardini</t>
         </is>
       </c>
       <c r="O91" t="inlineStr">
         <is>
-          <t>Maignan; Saelemaekers</t>
+          <t>Athekame; Estupinan</t>
         </is>
       </c>
       <c r="P91" t="inlineStr"/>
@@ -6582,23 +6582,23 @@
       <c r="J92" t="inlineStr"/>
       <c r="K92" t="inlineStr">
         <is>
-          <t>Soulè</t>
+          <t>Malen</t>
         </is>
       </c>
       <c r="L92" t="inlineStr"/>
       <c r="M92" t="inlineStr">
         <is>
-          <t>Malen</t>
+          <t>Zaragoza</t>
         </is>
       </c>
       <c r="N92" t="inlineStr">
         <is>
-          <t>Orsolini; Castro S.</t>
+          <t>De Silvestri; Lykogiannis</t>
         </is>
       </c>
       <c r="O92" t="inlineStr">
         <is>
-          <t>Svilar; Cristante</t>
+          <t>Zaragoza; Mancini</t>
         </is>
       </c>
       <c r="P92" t="inlineStr"/>
@@ -6647,23 +6647,23 @@
       <c r="J93" t="inlineStr"/>
       <c r="K93" t="inlineStr">
         <is>
-          <t>Raspadori</t>
+          <t>Scamacca</t>
         </is>
       </c>
       <c r="L93" t="inlineStr"/>
       <c r="M93" t="inlineStr">
         <is>
-          <t>Scamacca</t>
+          <t>Raspadori</t>
         </is>
       </c>
       <c r="N93" t="inlineStr">
         <is>
-          <t>Adopo; Caprile</t>
+          <t>Dossena; Obert</t>
         </is>
       </c>
       <c r="O93" t="inlineStr">
         <is>
-          <t>Carnesecchi; De Ketelaere</t>
+          <t>Kolasinac; De Roon</t>
         </is>
       </c>
       <c r="P93" t="inlineStr"/>
@@ -6711,7 +6711,7 @@
       </c>
       <c r="J94" t="inlineStr">
         <is>
-          <t>Brescianini</t>
+          <t>Kean</t>
         </is>
       </c>
       <c r="K94" t="inlineStr">
@@ -6721,22 +6721,22 @@
       </c>
       <c r="L94" t="inlineStr">
         <is>
-          <t>Mandragora</t>
+          <t>Harrison</t>
         </is>
       </c>
       <c r="M94" t="inlineStr">
         <is>
-          <t>Volpato</t>
+          <t>Garcia U.</t>
         </is>
       </c>
       <c r="N94" t="inlineStr">
         <is>
-          <t>De Gea; Dodò</t>
+          <t>Pongracic; Ranieri L.</t>
         </is>
       </c>
       <c r="O94" t="inlineStr">
         <is>
-          <t>Idzes; Laurientè</t>
+          <t>Iannoni; Thorstvedt</t>
         </is>
       </c>
       <c r="P94" t="inlineStr"/>
@@ -6785,23 +6785,23 @@
       <c r="J95" t="inlineStr"/>
       <c r="K95" t="inlineStr">
         <is>
-          <t>Baturina</t>
+          <t>Douvikas</t>
         </is>
       </c>
       <c r="L95" t="inlineStr"/>
       <c r="M95" t="inlineStr">
         <is>
-          <t>Paz N.</t>
+          <t>Baturina</t>
         </is>
       </c>
       <c r="N95" t="inlineStr">
         <is>
-          <t>Vasquez; Colombo</t>
+          <t>Gronbaek *; Malinovskyi</t>
         </is>
       </c>
       <c r="O95" t="inlineStr">
         <is>
-          <t>Butez; Paz N.</t>
+          <t>Smolcic I.; Diego Carlos</t>
         </is>
       </c>
       <c r="P95" t="inlineStr"/>
@@ -6849,29 +6849,29 @@
       </c>
       <c r="J96" t="inlineStr">
         <is>
-          <t>Castellanos *</t>
+          <t>Pedro</t>
         </is>
       </c>
       <c r="K96" t="inlineStr"/>
       <c r="L96" t="inlineStr">
         <is>
-          <t>Isaksen</t>
+          <t>Castellanos *</t>
         </is>
       </c>
       <c r="M96" t="inlineStr"/>
       <c r="N96" t="inlineStr">
         <is>
-          <t>Provedel; Gila</t>
+          <t>Taylor K.; Zaccagni</t>
         </is>
       </c>
       <c r="O96" t="inlineStr">
         <is>
-          <t>Karlstrom; Solet</t>
+          <t>Goglichidze *; Gueye</t>
         </is>
       </c>
       <c r="P96" t="inlineStr">
         <is>
-          <t>Basic</t>
+          <t>Belahyane</t>
         </is>
       </c>
       <c r="Q96" t="inlineStr"/>
@@ -6924,18 +6924,18 @@
       <c r="K97" t="inlineStr"/>
       <c r="L97" t="inlineStr">
         <is>
-          <t>Leao</t>
+          <t>Rabiot</t>
         </is>
       </c>
       <c r="M97" t="inlineStr"/>
       <c r="N97" t="inlineStr">
         <is>
-          <t>Maignan; Saelemaekers</t>
+          <t>Athekame; Estupinan</t>
         </is>
       </c>
       <c r="O97" t="inlineStr">
         <is>
-          <t>Kalulu</t>
+          <t>Gatti</t>
         </is>
       </c>
       <c r="P97" t="inlineStr"/>
@@ -6983,24 +6983,24 @@
       </c>
       <c r="J98" t="inlineStr">
         <is>
-          <t>De Bruyne</t>
+          <t>Santos A.</t>
         </is>
       </c>
       <c r="K98" t="inlineStr"/>
       <c r="L98" t="inlineStr">
         <is>
-          <t>Zambo Anguissa</t>
+          <t>Giovane</t>
         </is>
       </c>
       <c r="M98" t="inlineStr"/>
       <c r="N98" t="inlineStr">
         <is>
-          <t>Di Lorenzo</t>
+          <t>Juan Jesus</t>
         </is>
       </c>
       <c r="O98" t="inlineStr">
         <is>
-          <t>Baschirotto; Terracciano F.</t>
+          <t>Pezzella Giu.; Payero</t>
         </is>
       </c>
       <c r="P98" t="inlineStr"/>
@@ -7052,12 +7052,12 @@
       <c r="M99" t="inlineStr"/>
       <c r="N99" t="inlineStr">
         <is>
-          <t>Bernabè; Pellegrino M.</t>
+          <t>Rinaldi; Nicolussi Caviglia</t>
         </is>
       </c>
       <c r="O99" t="inlineStr">
         <is>
-          <t>Canestrelli; Aebischer</t>
+          <t>Coppola F.; Denoon</t>
         </is>
       </c>
       <c r="P99" t="inlineStr"/>
@@ -7106,23 +7106,23 @@
       <c r="J100" t="inlineStr"/>
       <c r="K100" t="inlineStr">
         <is>
-          <t>Martinez L.; Dimarco; Calhanoglu</t>
+          <t>Martinez L.; Calhanoglu; Thuram</t>
         </is>
       </c>
       <c r="L100" t="inlineStr"/>
       <c r="M100" t="inlineStr">
         <is>
-          <t>Bonny; Thuram</t>
+          <t>Dimarco; Barella</t>
         </is>
       </c>
       <c r="N100" t="inlineStr">
         <is>
-          <t>Lazaro; Vlasic</t>
+          <t>Aboukhlal; Nkounkou</t>
         </is>
       </c>
       <c r="O100" t="inlineStr">
         <is>
-          <t>Martinez L.; Barella</t>
+          <t>Calhanoglu; Barella</t>
         </is>
       </c>
       <c r="P100" t="inlineStr"/>
@@ -7174,12 +7174,12 @@
       <c r="M101" t="inlineStr"/>
       <c r="N101" t="inlineStr">
         <is>
-          <t>Bernede; Nelsson</t>
+          <t>Akpa Akpro; Gagliardini</t>
         </is>
       </c>
       <c r="O101" t="inlineStr">
         <is>
-          <t>Falcone; Gallo</t>
+          <t>Ramadani; Gaspar K.</t>
         </is>
       </c>
       <c r="P101" t="inlineStr"/>
@@ -7227,24 +7227,24 @@
       </c>
       <c r="J102" t="inlineStr">
         <is>
-          <t>Raspadori</t>
+          <t>Scamacca</t>
         </is>
       </c>
       <c r="K102" t="inlineStr"/>
       <c r="L102" t="inlineStr">
         <is>
-          <t>Scamacca</t>
+          <t>Raspadori</t>
         </is>
       </c>
       <c r="M102" t="inlineStr"/>
       <c r="N102" t="inlineStr">
         <is>
-          <t>Carnesecchi; De Ketelaere</t>
+          <t>Kolasinac; De Roon</t>
         </is>
       </c>
       <c r="O102" t="inlineStr">
         <is>
-          <t>Vasquez; Colombo</t>
+          <t>Gronbaek *; Malinovskyi</t>
         </is>
       </c>
       <c r="P102" t="inlineStr"/>
@@ -7302,22 +7302,22 @@
       </c>
       <c r="L103" t="inlineStr">
         <is>
-          <t>Orsolini</t>
+          <t>Dominguez B.</t>
         </is>
       </c>
       <c r="M103" t="inlineStr">
         <is>
-          <t>Kilicsoy</t>
+          <t>Mazzitelli</t>
         </is>
       </c>
       <c r="N103" t="inlineStr">
         <is>
-          <t>Orsolini; Castro S.</t>
+          <t>De Silvestri; Lykogiannis</t>
         </is>
       </c>
       <c r="O103" t="inlineStr">
         <is>
-          <t>Adopo; Caprile</t>
+          <t>Dossena; Obert</t>
         </is>
       </c>
       <c r="P103" t="inlineStr"/>
@@ -7365,24 +7365,24 @@
       </c>
       <c r="J104" t="inlineStr">
         <is>
-          <t>Baturina</t>
+          <t>Douvikas</t>
         </is>
       </c>
       <c r="K104" t="inlineStr"/>
       <c r="L104" t="inlineStr">
         <is>
-          <t>Paz N.</t>
+          <t>Baturina</t>
         </is>
       </c>
       <c r="M104" t="inlineStr"/>
       <c r="N104" t="inlineStr">
         <is>
-          <t>Butez; Paz N.</t>
+          <t>Smolcic I.; Diego Carlos</t>
         </is>
       </c>
       <c r="O104" t="inlineStr">
         <is>
-          <t>Di Lorenzo</t>
+          <t>Juan Jesus</t>
         </is>
       </c>
       <c r="P104" t="inlineStr"/>
@@ -7431,29 +7431,29 @@
       <c r="J105" t="inlineStr"/>
       <c r="K105" t="inlineStr">
         <is>
-          <t>Castellanos *</t>
+          <t>Pedro</t>
         </is>
       </c>
       <c r="L105" t="inlineStr"/>
       <c r="M105" t="inlineStr">
         <is>
-          <t>Isaksen</t>
+          <t>Castellanos *</t>
         </is>
       </c>
       <c r="N105" t="inlineStr">
         <is>
-          <t>Baschirotto; Terracciano F.</t>
+          <t>Pezzella Giu.; Payero</t>
         </is>
       </c>
       <c r="O105" t="inlineStr">
         <is>
-          <t>Provedel; Gila</t>
+          <t>Taylor K.; Zaccagni</t>
         </is>
       </c>
       <c r="P105" t="inlineStr"/>
       <c r="Q105" t="inlineStr">
         <is>
-          <t>Basic</t>
+          <t>Belahyane</t>
         </is>
       </c>
       <c r="R105" t="n">
@@ -7499,24 +7499,24 @@
       </c>
       <c r="J106" t="inlineStr">
         <is>
-          <t>Martinez L.; Dimarco</t>
+          <t>Martinez L.; Calhanoglu</t>
         </is>
       </c>
       <c r="K106" t="inlineStr"/>
       <c r="L106" t="inlineStr">
         <is>
-          <t>Calhanoglu; Bonny</t>
+          <t>Dimarco; Barella</t>
         </is>
       </c>
       <c r="M106" t="inlineStr"/>
       <c r="N106" t="inlineStr">
         <is>
-          <t>Martinez L.; Barella</t>
+          <t>Calhanoglu; Barella</t>
         </is>
       </c>
       <c r="O106" t="inlineStr">
         <is>
-          <t>Bernabè; Pellegrino M.</t>
+          <t>Rinaldi; Nicolussi Caviglia</t>
         </is>
       </c>
       <c r="P106" t="inlineStr"/>
@@ -7564,24 +7564,24 @@
       </c>
       <c r="J107" t="inlineStr">
         <is>
-          <t>Yildiz; Bremer</t>
+          <t>Yildiz; Kostic</t>
         </is>
       </c>
       <c r="K107" t="inlineStr"/>
       <c r="L107" t="inlineStr">
         <is>
-          <t>Kostic; Adzic</t>
+          <t>Boga; Holm</t>
         </is>
       </c>
       <c r="M107" t="inlineStr"/>
       <c r="N107" t="inlineStr">
         <is>
-          <t>Kalulu</t>
+          <t>Gatti</t>
         </is>
       </c>
       <c r="O107" t="inlineStr">
         <is>
-          <t>Bernede; Nelsson</t>
+          <t>Akpa Akpro; Gagliardini</t>
         </is>
       </c>
       <c r="P107" t="inlineStr"/>
@@ -7633,12 +7633,12 @@
       <c r="M108" t="inlineStr"/>
       <c r="N108" t="inlineStr">
         <is>
-          <t>Canestrelli; Aebischer</t>
+          <t>Coppola F.; Denoon</t>
         </is>
       </c>
       <c r="O108" t="inlineStr">
         <is>
-          <t>Falcone; Gallo</t>
+          <t>Ramadani; Gaspar K.</t>
         </is>
       </c>
       <c r="P108" t="inlineStr"/>
@@ -7686,24 +7686,24 @@
       </c>
       <c r="J109" t="inlineStr">
         <is>
-          <t>Soulè</t>
+          <t>Malen</t>
         </is>
       </c>
       <c r="K109" t="inlineStr"/>
       <c r="L109" t="inlineStr">
         <is>
-          <t>Malen</t>
+          <t>Zaragoza</t>
         </is>
       </c>
       <c r="M109" t="inlineStr"/>
       <c r="N109" t="inlineStr">
         <is>
-          <t>Svilar; Cristante</t>
+          <t>Zaragoza; Mancini</t>
         </is>
       </c>
       <c r="O109" t="inlineStr">
         <is>
-          <t>De Gea; Dodò</t>
+          <t>Pongracic; Ranieri L.</t>
         </is>
       </c>
       <c r="P109" t="inlineStr"/>
@@ -7758,17 +7758,17 @@
       <c r="L110" t="inlineStr"/>
       <c r="M110" t="inlineStr">
         <is>
-          <t>Leao</t>
+          <t>Rabiot</t>
         </is>
       </c>
       <c r="N110" t="inlineStr">
         <is>
-          <t>Idzes; Laurientè</t>
+          <t>Iannoni; Thorstvedt</t>
         </is>
       </c>
       <c r="O110" t="inlineStr">
         <is>
-          <t>Maignan; Saelemaekers</t>
+          <t>Athekame; Estupinan</t>
         </is>
       </c>
       <c r="P110" t="inlineStr"/>
@@ -7826,7 +7826,7 @@
       </c>
       <c r="L111" t="inlineStr">
         <is>
-          <t>Zaniolo</t>
+          <t>Rui Modesto *</t>
         </is>
       </c>
       <c r="M111" t="inlineStr">
@@ -7836,12 +7836,12 @@
       </c>
       <c r="N111" t="inlineStr">
         <is>
-          <t>Karlstrom; Solet</t>
+          <t>Goglichidze *; Gueye</t>
         </is>
       </c>
       <c r="O111" t="inlineStr">
         <is>
-          <t>Lazaro; Vlasic</t>
+          <t>Aboukhlal; Nkounkou</t>
         </is>
       </c>
       <c r="P111" t="inlineStr"/>
@@ -7899,22 +7899,22 @@
       </c>
       <c r="L112" t="inlineStr">
         <is>
-          <t>Kilicsoy</t>
+          <t>Mazzitelli</t>
         </is>
       </c>
       <c r="M112" t="inlineStr">
         <is>
-          <t>Zaniolo</t>
+          <t>Rui Modesto *</t>
         </is>
       </c>
       <c r="N112" t="inlineStr">
         <is>
-          <t>Adopo; Caprile</t>
+          <t>Dossena; Obert</t>
         </is>
       </c>
       <c r="O112" t="inlineStr">
         <is>
-          <t>Karlstrom; Solet</t>
+          <t>Goglichidze *; Gueye</t>
         </is>
       </c>
       <c r="P112" t="inlineStr"/>
@@ -7968,18 +7968,18 @@
       <c r="K113" t="inlineStr"/>
       <c r="L113" t="inlineStr">
         <is>
-          <t>Bonazzoli</t>
+          <t>Vandeputte</t>
         </is>
       </c>
       <c r="M113" t="inlineStr"/>
       <c r="N113" t="inlineStr">
         <is>
-          <t>Baschirotto; Terracciano F.</t>
+          <t>Pezzella Giu.; Payero</t>
         </is>
       </c>
       <c r="O113" t="inlineStr">
         <is>
-          <t>Canestrelli; Aebischer</t>
+          <t>Coppola F.; Denoon</t>
         </is>
       </c>
       <c r="P113" t="inlineStr"/>
@@ -8027,32 +8027,32 @@
       </c>
       <c r="J114" t="inlineStr">
         <is>
-          <t>Brescianini</t>
+          <t>Kean</t>
         </is>
       </c>
       <c r="K114" t="inlineStr">
         <is>
-          <t>Malinovskyi</t>
+          <t>Colombo</t>
         </is>
       </c>
       <c r="L114" t="inlineStr">
         <is>
-          <t>Mandragora</t>
+          <t>Harrison</t>
         </is>
       </c>
       <c r="M114" t="inlineStr">
         <is>
-          <t>Ostigard</t>
+          <t>Martin</t>
         </is>
       </c>
       <c r="N114" t="inlineStr">
         <is>
-          <t>De Gea; Dodò</t>
+          <t>Pongracic; Ranieri L.</t>
         </is>
       </c>
       <c r="O114" t="inlineStr">
         <is>
-          <t>Vasquez; Colombo</t>
+          <t>Gronbaek *; Malinovskyi</t>
         </is>
       </c>
       <c r="P114" t="inlineStr"/>
@@ -8112,17 +8112,17 @@
       </c>
       <c r="N115" t="inlineStr">
         <is>
-          <t>Provedel; Gila</t>
+          <t>Taylor K.; Zaccagni</t>
         </is>
       </c>
       <c r="O115" t="inlineStr">
         <is>
-          <t>Martinez L.; Barella</t>
+          <t>Calhanoglu; Barella</t>
         </is>
       </c>
       <c r="P115" t="inlineStr">
         <is>
-          <t>Basic</t>
+          <t>Belahyane</t>
         </is>
       </c>
       <c r="Q115" t="inlineStr"/>
@@ -8176,17 +8176,17 @@
       <c r="L116" t="inlineStr"/>
       <c r="M116" t="inlineStr">
         <is>
-          <t>Bremer</t>
+          <t>Boga</t>
         </is>
       </c>
       <c r="N116" t="inlineStr">
         <is>
-          <t>Falcone; Gallo</t>
+          <t>Ramadani; Gaspar K.</t>
         </is>
       </c>
       <c r="O116" t="inlineStr">
         <is>
-          <t>Kalulu</t>
+          <t>Gatti</t>
         </is>
       </c>
       <c r="P116" t="inlineStr"/>
@@ -8240,18 +8240,18 @@
       <c r="K117" t="inlineStr"/>
       <c r="L117" t="inlineStr">
         <is>
-          <t>Leao</t>
+          <t>Rabiot</t>
         </is>
       </c>
       <c r="M117" t="inlineStr"/>
       <c r="N117" t="inlineStr">
         <is>
-          <t>Maignan; Saelemaekers</t>
+          <t>Athekame; Estupinan</t>
         </is>
       </c>
       <c r="O117" t="inlineStr">
         <is>
-          <t>Carnesecchi; De Ketelaere</t>
+          <t>Kolasinac; De Roon</t>
         </is>
       </c>
       <c r="P117" t="inlineStr"/>
@@ -8299,24 +8299,24 @@
       </c>
       <c r="J118" t="inlineStr">
         <is>
-          <t>De Bruyne</t>
+          <t>Santos A.</t>
         </is>
       </c>
       <c r="K118" t="inlineStr"/>
       <c r="L118" t="inlineStr">
         <is>
-          <t>Zambo Anguissa</t>
+          <t>Giovane</t>
         </is>
       </c>
       <c r="M118" t="inlineStr"/>
       <c r="N118" t="inlineStr">
         <is>
-          <t>Di Lorenzo</t>
+          <t>Juan Jesus</t>
         </is>
       </c>
       <c r="O118" t="inlineStr">
         <is>
-          <t>Orsolini; Castro S.</t>
+          <t>De Silvestri; Lykogiannis</t>
         </is>
       </c>
       <c r="P118" t="inlineStr"/>
@@ -8365,23 +8365,23 @@
       <c r="J119" t="inlineStr"/>
       <c r="K119" t="inlineStr">
         <is>
-          <t>Soulè</t>
+          <t>Malen</t>
         </is>
       </c>
       <c r="L119" t="inlineStr"/>
       <c r="M119" t="inlineStr">
         <is>
-          <t>Malen</t>
+          <t>Zaragoza</t>
         </is>
       </c>
       <c r="N119" t="inlineStr">
         <is>
-          <t>Bernabè; Pellegrino M.</t>
+          <t>Rinaldi; Nicolussi Caviglia</t>
         </is>
       </c>
       <c r="O119" t="inlineStr">
         <is>
-          <t>Svilar; Cristante</t>
+          <t>Zaragoza; Mancini</t>
         </is>
       </c>
       <c r="P119" t="inlineStr"/>
@@ -8444,17 +8444,17 @@
       </c>
       <c r="M120" t="inlineStr">
         <is>
-          <t>Volpato</t>
+          <t>Garcia U.</t>
         </is>
       </c>
       <c r="N120" t="inlineStr">
         <is>
-          <t>Lazaro; Vlasic</t>
+          <t>Aboukhlal; Nkounkou</t>
         </is>
       </c>
       <c r="O120" t="inlineStr">
         <is>
-          <t>Idzes; Laurientè</t>
+          <t>Iannoni; Thorstvedt</t>
         </is>
       </c>
       <c r="P120" t="inlineStr"/>
@@ -8503,23 +8503,23 @@
       <c r="J121" t="inlineStr"/>
       <c r="K121" t="inlineStr">
         <is>
-          <t>Baturina; Paz N.</t>
+          <t>Douvikas; Baturina</t>
         </is>
       </c>
       <c r="L121" t="inlineStr"/>
       <c r="M121" t="inlineStr">
         <is>
-          <t>Douvikas; Kempf</t>
+          <t>Rodriguez Je.; Paz N.</t>
         </is>
       </c>
       <c r="N121" t="inlineStr">
         <is>
-          <t>Bernede; Nelsson</t>
+          <t>Akpa Akpro; Gagliardini</t>
         </is>
       </c>
       <c r="O121" t="inlineStr">
         <is>
-          <t>Butez; Paz N.</t>
+          <t>Smolcic I.; Diego Carlos</t>
         </is>
       </c>
       <c r="P121" t="inlineStr"/>
@@ -8567,24 +8567,24 @@
       </c>
       <c r="J122" t="inlineStr">
         <is>
-          <t>Raspadori</t>
+          <t>Scamacca</t>
         </is>
       </c>
       <c r="K122" t="inlineStr"/>
       <c r="L122" t="inlineStr">
         <is>
-          <t>Scamacca</t>
+          <t>Raspadori</t>
         </is>
       </c>
       <c r="M122" t="inlineStr"/>
       <c r="N122" t="inlineStr">
         <is>
-          <t>Carnesecchi; De Ketelaere</t>
+          <t>Kolasinac; De Roon</t>
         </is>
       </c>
       <c r="O122" t="inlineStr">
         <is>
-          <t>Orsolini; Castro S.</t>
+          <t>De Silvestri; Lykogiannis</t>
         </is>
       </c>
       <c r="P122" t="inlineStr"/>
@@ -8642,7 +8642,7 @@
       </c>
       <c r="L123" t="inlineStr">
         <is>
-          <t>Kilicsoy</t>
+          <t>Mazzitelli</t>
         </is>
       </c>
       <c r="M123" t="inlineStr">
@@ -8652,12 +8652,12 @@
       </c>
       <c r="N123" t="inlineStr">
         <is>
-          <t>Adopo; Caprile</t>
+          <t>Dossena; Obert</t>
         </is>
       </c>
       <c r="O123" t="inlineStr">
         <is>
-          <t>Lazaro; Vlasic</t>
+          <t>Aboukhlal; Nkounkou</t>
         </is>
       </c>
       <c r="P123" t="inlineStr"/>
@@ -8705,24 +8705,24 @@
       </c>
       <c r="J124" t="inlineStr">
         <is>
-          <t>Baturina</t>
+          <t>Douvikas</t>
         </is>
       </c>
       <c r="K124" t="inlineStr"/>
       <c r="L124" t="inlineStr">
         <is>
-          <t>Paz N.</t>
+          <t>Baturina</t>
         </is>
       </c>
       <c r="M124" t="inlineStr"/>
       <c r="N124" t="inlineStr">
         <is>
-          <t>Butez; Paz N.</t>
+          <t>Smolcic I.; Diego Carlos</t>
         </is>
       </c>
       <c r="O124" t="inlineStr">
         <is>
-          <t>Bernabè; Pellegrino M.</t>
+          <t>Rinaldi; Nicolussi Caviglia</t>
         </is>
       </c>
       <c r="P124" t="inlineStr"/>
@@ -8777,17 +8777,17 @@
       <c r="L125" t="inlineStr"/>
       <c r="M125" t="inlineStr">
         <is>
-          <t>Rabiot; Nkunku</t>
+          <t>Rabiot; Athekame</t>
         </is>
       </c>
       <c r="N125" t="inlineStr">
         <is>
-          <t>Vasquez; Colombo</t>
+          <t>Gronbaek *; Malinovskyi</t>
         </is>
       </c>
       <c r="O125" t="inlineStr">
         <is>
-          <t>Maignan; Saelemaekers</t>
+          <t>Athekame; Estupinan</t>
         </is>
       </c>
       <c r="P125" t="inlineStr"/>
@@ -8835,24 +8835,24 @@
       </c>
       <c r="J126" t="inlineStr">
         <is>
-          <t>Martinez L.; Dimarco; Calhanoglu</t>
+          <t>Martinez L.; Calhanoglu; Thuram</t>
         </is>
       </c>
       <c r="K126" t="inlineStr"/>
       <c r="L126" t="inlineStr">
         <is>
-          <t>Bonny; Thuram</t>
+          <t>Dimarco; Barella</t>
         </is>
       </c>
       <c r="M126" t="inlineStr"/>
       <c r="N126" t="inlineStr">
         <is>
-          <t>Martinez L.; Barella</t>
+          <t>Calhanoglu; Barella</t>
         </is>
       </c>
       <c r="O126" t="inlineStr">
         <is>
-          <t>Bernede; Nelsson</t>
+          <t>Akpa Akpro; Gagliardini</t>
         </is>
       </c>
       <c r="P126" t="inlineStr"/>
@@ -8900,24 +8900,24 @@
       </c>
       <c r="J127" t="inlineStr">
         <is>
-          <t>Yildiz; Bremer</t>
+          <t>Yildiz; Kostic</t>
         </is>
       </c>
       <c r="K127" t="inlineStr"/>
       <c r="L127" t="inlineStr">
         <is>
-          <t>Kostic; Adzic</t>
+          <t>Boga; Holm</t>
         </is>
       </c>
       <c r="M127" t="inlineStr"/>
       <c r="N127" t="inlineStr">
         <is>
-          <t>Kalulu</t>
+          <t>Gatti</t>
         </is>
       </c>
       <c r="O127" t="inlineStr">
         <is>
-          <t>De Gea; Dodò</t>
+          <t>Pongracic; Ranieri L.</t>
         </is>
       </c>
       <c r="P127" t="inlineStr"/>
@@ -8966,23 +8966,23 @@
       <c r="J128" t="inlineStr"/>
       <c r="K128" t="inlineStr">
         <is>
-          <t>De Bruyne</t>
+          <t>Santos A.</t>
         </is>
       </c>
       <c r="L128" t="inlineStr"/>
       <c r="M128" t="inlineStr">
         <is>
-          <t>Zambo Anguissa</t>
+          <t>Giovane</t>
         </is>
       </c>
       <c r="N128" t="inlineStr">
         <is>
-          <t>Canestrelli; Aebischer</t>
+          <t>Coppola F.; Denoon</t>
         </is>
       </c>
       <c r="O128" t="inlineStr">
         <is>
-          <t>Di Lorenzo</t>
+          <t>Juan Jesus</t>
         </is>
       </c>
       <c r="P128" t="inlineStr"/>
@@ -9030,30 +9030,30 @@
       </c>
       <c r="J129" t="inlineStr">
         <is>
-          <t>Soulè</t>
+          <t>Malen</t>
         </is>
       </c>
       <c r="K129" t="inlineStr"/>
       <c r="L129" t="inlineStr">
         <is>
-          <t>Malen</t>
+          <t>Zaragoza</t>
         </is>
       </c>
       <c r="M129" t="inlineStr"/>
       <c r="N129" t="inlineStr">
         <is>
-          <t>Svilar; Cristante</t>
+          <t>Zaragoza; Mancini</t>
         </is>
       </c>
       <c r="O129" t="inlineStr">
         <is>
-          <t>Provedel; Gila</t>
+          <t>Taylor K.; Zaccagni</t>
         </is>
       </c>
       <c r="P129" t="inlineStr"/>
       <c r="Q129" t="inlineStr">
         <is>
-          <t>Basic</t>
+          <t>Belahyane</t>
         </is>
       </c>
       <c r="R129" t="n">
@@ -9105,18 +9105,18 @@
       <c r="K130" t="inlineStr"/>
       <c r="L130" t="inlineStr">
         <is>
-          <t>Volpato</t>
+          <t>Garcia U.</t>
         </is>
       </c>
       <c r="M130" t="inlineStr"/>
       <c r="N130" t="inlineStr">
         <is>
-          <t>Idzes; Laurientè</t>
+          <t>Iannoni; Thorstvedt</t>
         </is>
       </c>
       <c r="O130" t="inlineStr">
         <is>
-          <t>Falcone; Gallo</t>
+          <t>Ramadani; Gaspar K.</t>
         </is>
       </c>
       <c r="P130" t="inlineStr"/>
@@ -9174,22 +9174,22 @@
       </c>
       <c r="L131" t="inlineStr">
         <is>
-          <t>Zaniolo</t>
+          <t>Rui Modesto *</t>
         </is>
       </c>
       <c r="M131" t="inlineStr">
         <is>
-          <t>Bonazzoli</t>
+          <t>Vandeputte</t>
         </is>
       </c>
       <c r="N131" t="inlineStr">
         <is>
-          <t>Karlstrom; Solet</t>
+          <t>Goglichidze *; Gueye</t>
         </is>
       </c>
       <c r="O131" t="inlineStr">
         <is>
-          <t>Baschirotto; Terracciano F.</t>
+          <t>Pezzella Giu.; Payero</t>
         </is>
       </c>
       <c r="P131" t="inlineStr"/>
@@ -9238,23 +9238,23 @@
       <c r="J132" t="inlineStr"/>
       <c r="K132" t="inlineStr">
         <is>
-          <t>Martinez L.; Dimarco</t>
+          <t>Martinez L.; Calhanoglu</t>
         </is>
       </c>
       <c r="L132" t="inlineStr"/>
       <c r="M132" t="inlineStr">
         <is>
-          <t>Calhanoglu; Bonny</t>
+          <t>Dimarco; Barella</t>
         </is>
       </c>
       <c r="N132" t="inlineStr">
         <is>
-          <t>Orsolini; Castro S.</t>
+          <t>De Silvestri; Lykogiannis</t>
         </is>
       </c>
       <c r="O132" t="inlineStr">
         <is>
-          <t>Martinez L.; Barella</t>
+          <t>Calhanoglu; Barella</t>
         </is>
       </c>
       <c r="P132" t="inlineStr"/>
@@ -9303,23 +9303,23 @@
       <c r="J133" t="inlineStr"/>
       <c r="K133" t="inlineStr">
         <is>
-          <t>Baturina</t>
+          <t>Douvikas</t>
         </is>
       </c>
       <c r="L133" t="inlineStr"/>
       <c r="M133" t="inlineStr">
         <is>
-          <t>Paz N.</t>
+          <t>Baturina</t>
         </is>
       </c>
       <c r="N133" t="inlineStr">
         <is>
-          <t>Baschirotto; Terracciano F.</t>
+          <t>Pezzella Giu.; Payero</t>
         </is>
       </c>
       <c r="O133" t="inlineStr">
         <is>
-          <t>Butez; Paz N.</t>
+          <t>Smolcic I.; Diego Carlos</t>
         </is>
       </c>
       <c r="P133" t="inlineStr"/>
@@ -9368,23 +9368,23 @@
       <c r="J134" t="inlineStr"/>
       <c r="K134" t="inlineStr">
         <is>
-          <t>Raspadori</t>
+          <t>Scamacca</t>
         </is>
       </c>
       <c r="L134" t="inlineStr"/>
       <c r="M134" t="inlineStr">
         <is>
-          <t>Scamacca</t>
+          <t>Raspadori</t>
         </is>
       </c>
       <c r="N134" t="inlineStr">
         <is>
-          <t>De Gea; Dodò</t>
+          <t>Pongracic; Ranieri L.</t>
         </is>
       </c>
       <c r="O134" t="inlineStr">
         <is>
-          <t>Carnesecchi; De Ketelaere</t>
+          <t>Kolasinac; De Roon</t>
         </is>
       </c>
       <c r="P134" t="inlineStr"/>
@@ -9432,29 +9432,29 @@
       </c>
       <c r="J135" t="inlineStr">
         <is>
-          <t>Castellanos *</t>
+          <t>Pedro</t>
         </is>
       </c>
       <c r="K135" t="inlineStr"/>
       <c r="L135" t="inlineStr">
         <is>
-          <t>Isaksen</t>
+          <t>Castellanos *</t>
         </is>
       </c>
       <c r="M135" t="inlineStr"/>
       <c r="N135" t="inlineStr">
         <is>
-          <t>Provedel; Gila</t>
+          <t>Taylor K.; Zaccagni</t>
         </is>
       </c>
       <c r="O135" t="inlineStr">
         <is>
-          <t>Canestrelli; Aebischer</t>
+          <t>Coppola F.; Denoon</t>
         </is>
       </c>
       <c r="P135" t="inlineStr">
         <is>
-          <t>Basic</t>
+          <t>Belahyane</t>
         </is>
       </c>
       <c r="Q135" t="inlineStr"/>
@@ -9502,23 +9502,23 @@
       <c r="J136" t="inlineStr"/>
       <c r="K136" t="inlineStr">
         <is>
-          <t>Malinovskyi</t>
+          <t>Colombo</t>
         </is>
       </c>
       <c r="L136" t="inlineStr"/>
       <c r="M136" t="inlineStr">
         <is>
-          <t>Ostigard</t>
+          <t>Martin</t>
         </is>
       </c>
       <c r="N136" t="inlineStr">
         <is>
-          <t>Falcone; Gallo</t>
+          <t>Ramadani; Gaspar K.</t>
         </is>
       </c>
       <c r="O136" t="inlineStr">
         <is>
-          <t>Vasquez; Colombo</t>
+          <t>Gronbaek *; Malinovskyi</t>
         </is>
       </c>
       <c r="P136" t="inlineStr"/>
@@ -9572,18 +9572,18 @@
       <c r="K137" t="inlineStr"/>
       <c r="L137" t="inlineStr">
         <is>
-          <t>Leao</t>
+          <t>Rabiot</t>
         </is>
       </c>
       <c r="M137" t="inlineStr"/>
       <c r="N137" t="inlineStr">
         <is>
-          <t>Maignan; Saelemaekers</t>
+          <t>Athekame; Estupinan</t>
         </is>
       </c>
       <c r="O137" t="inlineStr">
         <is>
-          <t>Adopo; Caprile</t>
+          <t>Dossena; Obert</t>
         </is>
       </c>
       <c r="P137" t="inlineStr"/>
@@ -9631,24 +9631,24 @@
       </c>
       <c r="J138" t="inlineStr">
         <is>
-          <t>De Bruyne; Zambo Anguissa</t>
+          <t>Santos A.; De Bruyne</t>
         </is>
       </c>
       <c r="K138" t="inlineStr"/>
       <c r="L138" t="inlineStr">
         <is>
-          <t>Vergara; McTominay</t>
+          <t>Giovane; Neres</t>
         </is>
       </c>
       <c r="M138" t="inlineStr"/>
       <c r="N138" t="inlineStr">
         <is>
-          <t>Di Lorenzo</t>
+          <t>Juan Jesus</t>
         </is>
       </c>
       <c r="O138" t="inlineStr">
         <is>
-          <t>Karlstrom; Solet</t>
+          <t>Goglichidze *; Gueye</t>
         </is>
       </c>
       <c r="P138" t="inlineStr"/>
@@ -9703,17 +9703,17 @@
       <c r="L139" t="inlineStr"/>
       <c r="M139" t="inlineStr">
         <is>
-          <t>Volpato</t>
+          <t>Garcia U.</t>
         </is>
       </c>
       <c r="N139" t="inlineStr">
         <is>
-          <t>Bernabè; Pellegrino M.</t>
+          <t>Rinaldi; Nicolussi Caviglia</t>
         </is>
       </c>
       <c r="O139" t="inlineStr">
         <is>
-          <t>Idzes; Laurientè</t>
+          <t>Iannoni; Thorstvedt</t>
         </is>
       </c>
       <c r="P139" t="inlineStr"/>
@@ -9762,23 +9762,23 @@
       <c r="J140" t="inlineStr"/>
       <c r="K140" t="inlineStr">
         <is>
-          <t>Yildiz; Bremer</t>
+          <t>Yildiz; Kostic</t>
         </is>
       </c>
       <c r="L140" t="inlineStr"/>
       <c r="M140" t="inlineStr">
         <is>
-          <t>Kostic; Adzic</t>
+          <t>Boga; Holm</t>
         </is>
       </c>
       <c r="N140" t="inlineStr">
         <is>
-          <t>Lazaro; Vlasic</t>
+          <t>Aboukhlal; Nkounkou</t>
         </is>
       </c>
       <c r="O140" t="inlineStr">
         <is>
-          <t>Kalulu</t>
+          <t>Gatti</t>
         </is>
       </c>
       <c r="P140" t="inlineStr"/>
@@ -9827,23 +9827,23 @@
       <c r="J141" t="inlineStr"/>
       <c r="K141" t="inlineStr">
         <is>
-          <t>Soulè</t>
+          <t>Malen</t>
         </is>
       </c>
       <c r="L141" t="inlineStr"/>
       <c r="M141" t="inlineStr">
         <is>
-          <t>Malen</t>
+          <t>Zaragoza</t>
         </is>
       </c>
       <c r="N141" t="inlineStr">
         <is>
-          <t>Bernede; Nelsson</t>
+          <t>Akpa Akpro; Gagliardini</t>
         </is>
       </c>
       <c r="O141" t="inlineStr">
         <is>
-          <t>Svilar; Cristante</t>
+          <t>Zaragoza; Mancini</t>
         </is>
       </c>
       <c r="P141" t="inlineStr"/>

</xml_diff>